<commit_message>
Update the excel sheets with alignment percentages
</commit_message>
<xml_diff>
--- a/group10.Code/analysis/Data Analysis Amazon.xlsx
+++ b/group10.Code/analysis/Data Analysis Amazon.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="98">
   <si>
     <t>Total</t>
   </si>
@@ -61,139 +61,142 @@
     <t>Rating vs Sentiment Matrix</t>
   </si>
   <si>
+    <t>🠗 Sentiment</t>
+  </si>
+  <si>
+    <t>Sentiment</t>
+  </si>
+  <si>
     <t>🠖 Score</t>
   </si>
   <si>
-    <t>🠗 Sentiment</t>
-  </si>
-  <si>
-    <t>13  6  15  10  19</t>
-  </si>
-  <si>
-    <t>121  95  69  71  138</t>
-  </si>
-  <si>
-    <t>497  465  749  1154  2824</t>
-  </si>
-  <si>
-    <t>79  110  427  1486  5422</t>
-  </si>
-  <si>
-    <t>15  8  65  254  1235</t>
-  </si>
-  <si>
-    <t>2  2  2  2  6</t>
-  </si>
-  <si>
-    <t>16  14  7  5  16</t>
-  </si>
-  <si>
-    <t>49  43  75  145  330</t>
-  </si>
-  <si>
-    <t>6  9  54  170  658</t>
-  </si>
-  <si>
-    <t>4  1  13  44  184</t>
-  </si>
-  <si>
-    <t>2  0  2  0  3</t>
-  </si>
-  <si>
-    <t>10  4  5  6  13</t>
-  </si>
-  <si>
-    <t>31  42  69  130  387</t>
-  </si>
-  <si>
-    <t>7  7  33  206  733</t>
-  </si>
-  <si>
-    <t>0  1  3  22  124</t>
-  </si>
-  <si>
-    <t>0  1  2  0  2</t>
-  </si>
-  <si>
-    <t>8  7  2  3  10</t>
-  </si>
-  <si>
-    <t>20  25  72  161  371</t>
-  </si>
-  <si>
-    <t>6  11  40  239  738</t>
-  </si>
-  <si>
-    <t>2  0  4  23  124</t>
-  </si>
-  <si>
-    <t>7  1  7  7  8</t>
-  </si>
-  <si>
-    <t>46  29  36  38  74</t>
-  </si>
-  <si>
-    <t>149  138  227  325  751</t>
-  </si>
-  <si>
-    <t>30  32  120  329  1225</t>
-  </si>
-  <si>
-    <t>3  3  21  79  342</t>
-  </si>
-  <si>
-    <t>0  0  0  0  0</t>
-  </si>
-  <si>
-    <t>15  10  6  9  12</t>
-  </si>
-  <si>
-    <t>128  71  110  166  432</t>
-  </si>
-  <si>
-    <t>12  13  48  182  711</t>
-  </si>
-  <si>
-    <t>4  0  3  23  132</t>
-  </si>
-  <si>
-    <t>0  2  0  1  0</t>
-  </si>
-  <si>
-    <t>8  12  7  7  2</t>
-  </si>
-  <si>
-    <t>43  63  82  118  245</t>
-  </si>
-  <si>
-    <t>8  22  70  192  751</t>
-  </si>
-  <si>
-    <t>1  1  6  38  229</t>
-  </si>
-  <si>
-    <t>2  0  2  0  0</t>
-  </si>
-  <si>
-    <t>18  19  6  3  11</t>
-  </si>
-  <si>
-    <t>77  83  114  109  308</t>
-  </si>
-  <si>
-    <t>10  16  62  168  606</t>
-  </si>
-  <si>
-    <t>1  2  15  25  100</t>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>13  121  497  79  15</t>
+  </si>
+  <si>
+    <t>6  95  465  110  8</t>
+  </si>
+  <si>
+    <t>15  69  749  427  65</t>
+  </si>
+  <si>
+    <t>10  71  1154  1486  254</t>
+  </si>
+  <si>
+    <t>19  138  2824  5422  1235</t>
+  </si>
+  <si>
+    <t>2  16  49  6  4</t>
+  </si>
+  <si>
+    <t>2  14  43  9  1</t>
+  </si>
+  <si>
+    <t>2  7  75  54  13</t>
+  </si>
+  <si>
+    <t>2  5  145  170  44</t>
+  </si>
+  <si>
+    <t>6  16  330  658  184</t>
+  </si>
+  <si>
+    <t>2  10  31  7  0</t>
+  </si>
+  <si>
+    <t>0  4  42  7  1</t>
+  </si>
+  <si>
+    <t>2  5  69  33  3</t>
+  </si>
+  <si>
+    <t>0  6  130  206  22</t>
+  </si>
+  <si>
+    <t>3  13  387  733  124</t>
+  </si>
+  <si>
+    <t>0  8  20  6  2</t>
+  </si>
+  <si>
+    <t>1  7  25  11  0</t>
+  </si>
+  <si>
+    <t>2  2  72  40  4</t>
+  </si>
+  <si>
+    <t>0  3  161  239  23</t>
+  </si>
+  <si>
+    <t>2  10  371  738  124</t>
+  </si>
+  <si>
+    <t>7  46  149  30  3</t>
+  </si>
+  <si>
+    <t>1  29  138  32  3</t>
+  </si>
+  <si>
+    <t>7  36  227  120  21</t>
+  </si>
+  <si>
+    <t>7  38  325  329  79</t>
+  </si>
+  <si>
+    <t>8  74  751  1225  342</t>
+  </si>
+  <si>
+    <t>0  15  128  12  4</t>
+  </si>
+  <si>
+    <t>0  10  71  13  0</t>
+  </si>
+  <si>
+    <t>0  6  110  48  3</t>
+  </si>
+  <si>
+    <t>0  9  166  182  23</t>
+  </si>
+  <si>
+    <t>0  12  432  711  132</t>
+  </si>
+  <si>
+    <t>0  8  43  8  1</t>
+  </si>
+  <si>
+    <t>2  12  63  22  1</t>
+  </si>
+  <si>
+    <t>0  7  82  70  6</t>
+  </si>
+  <si>
+    <t>1  7  118  192  38</t>
+  </si>
+  <si>
+    <t>0  2  245  751  229</t>
+  </si>
+  <si>
+    <t>2  18  77  10  1</t>
+  </si>
+  <si>
+    <t>0  19  83  16  2</t>
+  </si>
+  <si>
+    <t>2  6  114  62  15</t>
+  </si>
+  <si>
+    <t>0  3  109  168  25</t>
+  </si>
+  <si>
+    <t>0  11  308  606  100</t>
   </si>
   <si>
     <t>Graphs</t>
   </si>
   <si>
     <t xml:space="preserve"> Walmart Data Analysis Graphs will be located in another excel sheet.</t>
-  </si>
-  <si>
-    <t>Sentiment</t>
   </si>
   <si>
     <t>Estimated Score</t>
@@ -308,7 +311,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -336,6 +339,9 @@
     <font>
       <b/>
       <color rgb="FFAEAEAE"/>
+    </font>
+    <font>
+      <b/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -395,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -427,11 +433,26 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1717,13 +1738,23 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30">
-      <c r="C30" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="C30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
     </row>
     <row r="31">
-      <c r="A31" s="10" t="s">
-        <v>16</v>
+      <c r="B31" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="C31" s="2">
         <v>1.0</v>
@@ -1740,65 +1771,126 @@
       <c r="G31" s="2">
         <v>5.0</v>
       </c>
+      <c r="J31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="L31" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="M31" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="N31" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="O31" s="13">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="B32" s="2">
         <v>1.0</v>
       </c>
       <c r="C32" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K32, ""      "")"),13.0)</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H32, ""      "")"),13.0)</f>
         <v>13</v>
       </c>
-      <c r="D32" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
-        <v>6</v>
-      </c>
-      <c r="E32" s="11">
+      <c r="D32" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),121.0)</f>
+        <v>121</v>
+      </c>
+      <c r="E32" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),497.0)</f>
+        <v>497</v>
+      </c>
+      <c r="F32" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),79.0)</f>
+        <v>79</v>
+      </c>
+      <c r="G32" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),15.0)</f>
         <v>15</v>
       </c>
-      <c r="F32" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.0)</f>
-        <v>10</v>
-      </c>
-      <c r="G32" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),19.0)</f>
-        <v>19</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>18</v>
+      <c r="H32" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="K32" s="5" t="str">
+        <f t="shared" ref="K32:O32" si="17">ROUNDUP((C32/$K5), 4)*100&amp;"%"</f>
+        <v>1.75%</v>
+      </c>
+      <c r="L32" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>16.29%</v>
+      </c>
+      <c r="M32" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>66.9%</v>
+      </c>
+      <c r="N32" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>10.64%</v>
+      </c>
+      <c r="O32" s="5" t="str">
+        <f t="shared" si="17"/>
+        <v>2.02%</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="13"/>
+      <c r="A33" s="17"/>
       <c r="B33" s="2">
         <v>2.0</v>
       </c>
       <c r="C33" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K33, ""      "")"),121.0)</f>
-        <v>121</v>
-      </c>
-      <c r="D33" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H33, ""      "")"),6.0)</f>
+        <v>6</v>
+      </c>
+      <c r="D33" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),95.0)</f>
         <v>95</v>
       </c>
-      <c r="E33" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),69.0)</f>
-        <v>69</v>
-      </c>
-      <c r="F33" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),71.0)</f>
-        <v>71</v>
-      </c>
-      <c r="G33" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),138.0)</f>
-        <v>138</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>19</v>
+      <c r="E33" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),465.0)</f>
+        <v>465</v>
+      </c>
+      <c r="F33" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),110.0)</f>
+        <v>110</v>
+      </c>
+      <c r="G33" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),8.0)</f>
+        <v>8</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="K33" s="5" t="str">
+        <f t="shared" ref="K33:O33" si="18">ROUNDUP((C33/$K6), 4)*100&amp;"%"</f>
+        <v>0.87%</v>
+      </c>
+      <c r="L33" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>13.69%</v>
+      </c>
+      <c r="M33" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>67.01%</v>
+      </c>
+      <c r="N33" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>15.86%</v>
+      </c>
+      <c r="O33" s="5" t="str">
+        <f t="shared" si="18"/>
+        <v>1.16%</v>
       </c>
     </row>
     <row r="34">
@@ -1807,27 +1899,50 @@
         <v>3.0</v>
       </c>
       <c r="C34" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K34, ""      "")"),497.0)</f>
-        <v>497</v>
-      </c>
-      <c r="D34" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),465.0)</f>
-        <v>465</v>
-      </c>
-      <c r="E34" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H34, ""      "")"),15.0)</f>
+        <v>15</v>
+      </c>
+      <c r="D34" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),69.0)</f>
+        <v>69</v>
+      </c>
+      <c r="E34" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),749.0)</f>
         <v>749</v>
       </c>
-      <c r="F34" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1154.0)</f>
-        <v>1154</v>
-      </c>
-      <c r="G34" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2824.0)</f>
-        <v>2824</v>
-      </c>
-      <c r="K34" s="12" t="s">
-        <v>20</v>
+      <c r="F34" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),427.0)</f>
+        <v>427</v>
+      </c>
+      <c r="G34" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),65.0)</f>
+        <v>65</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="K34" s="5" t="str">
+        <f t="shared" ref="K34:O34" si="19">ROUNDUP((C34/$K7), 4)*100&amp;"%"</f>
+        <v>1.1%</v>
+      </c>
+      <c r="L34" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>5.06%</v>
+      </c>
+      <c r="M34" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>54.92%</v>
+      </c>
+      <c r="N34" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>31.31%</v>
+      </c>
+      <c r="O34" s="5" t="str">
+        <f t="shared" si="19"/>
+        <v>4.77%</v>
       </c>
     </row>
     <row r="35">
@@ -1836,27 +1951,50 @@
         <v>4.0</v>
       </c>
       <c r="C35" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K35, ""      "")"),79.0)</f>
-        <v>79</v>
-      </c>
-      <c r="D35" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),110.0)</f>
-        <v>110</v>
-      </c>
-      <c r="E35" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),427.0)</f>
-        <v>427</v>
-      </c>
-      <c r="F35" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H35, ""      "")"),10.0)</f>
+        <v>10</v>
+      </c>
+      <c r="D35" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),71.0)</f>
+        <v>71</v>
+      </c>
+      <c r="E35" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1154.0)</f>
+        <v>1154</v>
+      </c>
+      <c r="F35" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1486.0)</f>
         <v>1486</v>
       </c>
-      <c r="G35" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5422.0)</f>
-        <v>5422</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>21</v>
+      <c r="G35" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),254.0)</f>
+        <v>254</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="K35" s="5" t="str">
+        <f t="shared" ref="K35:O35" si="20">ROUNDUP((C35/$K8), 4)*100&amp;"%"</f>
+        <v>0.34%</v>
+      </c>
+      <c r="L35" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>2.35%</v>
+      </c>
+      <c r="M35" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>38.09%</v>
+      </c>
+      <c r="N35" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>49.05%</v>
+      </c>
+      <c r="O35" s="5" t="str">
+        <f t="shared" si="20"/>
+        <v>8.39%</v>
       </c>
     </row>
     <row r="36">
@@ -1865,40 +2003,73 @@
         <v>5.0</v>
       </c>
       <c r="C36" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K36, ""      "")"),15.0)</f>
-        <v>15</v>
-      </c>
-      <c r="D36" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),8.0)</f>
-        <v>8</v>
-      </c>
-      <c r="E36" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),65.0)</f>
-        <v>65</v>
-      </c>
-      <c r="F36" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),254.0)</f>
-        <v>254</v>
-      </c>
-      <c r="G36" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H36, ""      "")"),19.0)</f>
+        <v>19</v>
+      </c>
+      <c r="D36" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),138.0)</f>
+        <v>138</v>
+      </c>
+      <c r="E36" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2824.0)</f>
+        <v>2824</v>
+      </c>
+      <c r="F36" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5422.0)</f>
+        <v>5422</v>
+      </c>
+      <c r="G36" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1235.0)</f>
         <v>1235</v>
       </c>
-      <c r="K36" s="12" t="s">
-        <v>22</v>
+      <c r="H36" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="K36" s="5" t="str">
+        <f t="shared" ref="K36:O36" si="21">ROUNDUP((C36/$K9), 4)*100&amp;"%"</f>
+        <v>0.2%</v>
+      </c>
+      <c r="L36" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>1.4%</v>
+      </c>
+      <c r="M36" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>28.56%</v>
+      </c>
+      <c r="N36" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>54.83%</v>
+      </c>
+      <c r="O36" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>12.49%</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5"/>
     </row>
     <row r="38">
-      <c r="C38" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
     </row>
     <row r="39">
-      <c r="A39" s="10" t="s">
-        <v>16</v>
+      <c r="B39" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="C39" s="2">
         <v>1.0</v>
@@ -1915,65 +2086,126 @@
       <c r="G39" s="2">
         <v>5.0</v>
       </c>
+      <c r="J39" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="L39" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="M39" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="N39" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="O39" s="13">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="B40" s="2">
         <v>1.0</v>
       </c>
       <c r="C40" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K40, ""      "")"),2.0)</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H40, ""      "")"),2.0)</f>
         <v>2</v>
       </c>
-      <c r="D40" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
-      </c>
-      <c r="E40" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
-      </c>
-      <c r="F40" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
-      </c>
-      <c r="G40" s="11">
+      <c r="D40" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),16.0)</f>
+        <v>16</v>
+      </c>
+      <c r="E40" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),49.0)</f>
+        <v>49</v>
+      </c>
+      <c r="F40" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
         <v>6</v>
       </c>
-      <c r="K40" s="12" t="s">
-        <v>23</v>
+      <c r="G40" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.0)</f>
+        <v>4</v>
+      </c>
+      <c r="H40" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J40" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="K40" s="5" t="str">
+        <f t="shared" ref="K40:O40" si="22">ROUNDUP((C40/$L5), 4)*100&amp;"%"</f>
+        <v>2.6%</v>
+      </c>
+      <c r="L40" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>20.78%</v>
+      </c>
+      <c r="M40" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>63.64%</v>
+      </c>
+      <c r="N40" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>7.8%</v>
+      </c>
+      <c r="O40" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>5.2%</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="13"/>
+      <c r="A41" s="17"/>
       <c r="B41" s="2">
         <v>2.0</v>
       </c>
       <c r="C41" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K41, ""      "")"),16.0)</f>
-        <v>16</v>
-      </c>
-      <c r="D41" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H41, ""      "")"),2.0)</f>
+        <v>2</v>
+      </c>
+      <c r="D41" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),14.0)</f>
         <v>14</v>
       </c>
-      <c r="E41" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
-        <v>7</v>
-      </c>
-      <c r="F41" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.0)</f>
-        <v>5</v>
-      </c>
-      <c r="G41" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),16.0)</f>
-        <v>16</v>
-      </c>
-      <c r="K41" s="12" t="s">
-        <v>24</v>
+      <c r="E41" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43.0)</f>
+        <v>43</v>
+      </c>
+      <c r="F41" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),9.0)</f>
+        <v>9</v>
+      </c>
+      <c r="G41" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J41" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="K41" s="5" t="str">
+        <f t="shared" ref="K41:O41" si="23">ROUNDUP((C41/$L6), 4)*100&amp;"%"</f>
+        <v>2.86%</v>
+      </c>
+      <c r="L41" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>20%</v>
+      </c>
+      <c r="M41" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>61.43%</v>
+      </c>
+      <c r="N41" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>12.86%</v>
+      </c>
+      <c r="O41" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>1.43%</v>
       </c>
     </row>
     <row r="42">
@@ -1982,27 +2214,50 @@
         <v>3.0</v>
       </c>
       <c r="C42" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K42, ""      "")"),49.0)</f>
-        <v>49</v>
-      </c>
-      <c r="D42" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43.0)</f>
-        <v>43</v>
-      </c>
-      <c r="E42" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H42, ""      "")"),2.0)</f>
+        <v>2</v>
+      </c>
+      <c r="D42" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
+        <v>7</v>
+      </c>
+      <c r="E42" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),75.0)</f>
         <v>75</v>
       </c>
-      <c r="F42" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),145.0)</f>
-        <v>145</v>
-      </c>
-      <c r="G42" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),330.0)</f>
-        <v>330</v>
-      </c>
-      <c r="K42" s="12" t="s">
-        <v>25</v>
+      <c r="F42" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),54.0)</f>
+        <v>54</v>
+      </c>
+      <c r="G42" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.0)</f>
+        <v>13</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J42" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="K42" s="5" t="str">
+        <f t="shared" ref="K42:O42" si="24">ROUNDUP((C42/$L7), 4)*100&amp;"%"</f>
+        <v>1.27%</v>
+      </c>
+      <c r="L42" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>4.44%</v>
+      </c>
+      <c r="M42" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>47.47%</v>
+      </c>
+      <c r="N42" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>34.18%</v>
+      </c>
+      <c r="O42" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>8.23%</v>
       </c>
     </row>
     <row r="43">
@@ -2011,27 +2266,50 @@
         <v>4.0</v>
       </c>
       <c r="C43" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K43, ""      "")"),6.0)</f>
-        <v>6</v>
-      </c>
-      <c r="D43" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),9.0)</f>
-        <v>9</v>
-      </c>
-      <c r="E43" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),54.0)</f>
-        <v>54</v>
-      </c>
-      <c r="F43" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H43, ""      "")"),2.0)</f>
+        <v>2</v>
+      </c>
+      <c r="D43" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.0)</f>
+        <v>5</v>
+      </c>
+      <c r="E43" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),145.0)</f>
+        <v>145</v>
+      </c>
+      <c r="F43" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),170.0)</f>
         <v>170</v>
       </c>
-      <c r="G43" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),658.0)</f>
-        <v>658</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>26</v>
+      <c r="G43" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44.0)</f>
+        <v>44</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J43" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="K43" s="5" t="str">
+        <f t="shared" ref="K43:O43" si="25">ROUNDUP((C43/$L8), 4)*100&amp;"%"</f>
+        <v>0.54%</v>
+      </c>
+      <c r="L43" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>1.34%</v>
+      </c>
+      <c r="M43" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>38.78%</v>
+      </c>
+      <c r="N43" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>45.46%</v>
+      </c>
+      <c r="O43" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>11.77%</v>
       </c>
     </row>
     <row r="44">
@@ -2040,115 +2318,209 @@
         <v>5.0</v>
       </c>
       <c r="C44" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K44, ""      "")"),4.0)</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H44, ""      "")"),6.0)</f>
+        <v>6</v>
+      </c>
+      <c r="D44" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),16.0)</f>
+        <v>16</v>
+      </c>
+      <c r="E44" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),330.0)</f>
+        <v>330</v>
+      </c>
+      <c r="F44" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),658.0)</f>
+        <v>658</v>
+      </c>
+      <c r="G44" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),184.0)</f>
+        <v>184</v>
+      </c>
+      <c r="H44" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J44" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="K44" s="5" t="str">
+        <f t="shared" ref="K44:O44" si="26">ROUNDUP((C44/$L9), 4)*100&amp;"%"</f>
+        <v>0.5%</v>
+      </c>
+      <c r="L44" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>1.31%</v>
+      </c>
+      <c r="M44" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>26.97%</v>
+      </c>
+      <c r="N44" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>53.76%</v>
+      </c>
+      <c r="O44" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>15.04%</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="5"/>
+    </row>
+    <row r="46">
+      <c r="B46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K46" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+    </row>
+    <row r="47">
+      <c r="B47" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D47" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E47" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F47" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="G47" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="J47" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K47" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="L47" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="M47" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="N47" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="O47" s="13">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C48" s="8">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H48, ""      "")"),2.0)</f>
+        <v>2</v>
+      </c>
+      <c r="D48" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.0)</f>
+        <v>10</v>
+      </c>
+      <c r="E48" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),31.0)</f>
+        <v>31</v>
+      </c>
+      <c r="F48" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
+        <v>7</v>
+      </c>
+      <c r="G48" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J48" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="K48" s="5" t="str">
+        <f t="shared" ref="K48:O48" si="27">ROUNDUP((C48/$M5), 4)*100&amp;"%"</f>
+        <v>3.93%</v>
+      </c>
+      <c r="L48" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>19.61%</v>
+      </c>
+      <c r="M48" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>60.79%</v>
+      </c>
+      <c r="N48" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>13.73%</v>
+      </c>
+      <c r="O48" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>0%</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="17"/>
+      <c r="B49" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="C49" s="8">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H49, ""      "")"),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="D49" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.0)</f>
         <v>4</v>
       </c>
-      <c r="D44" s="11">
+      <c r="E49" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),42.0)</f>
+        <v>42</v>
+      </c>
+      <c r="F49" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
+        <v>7</v>
+      </c>
+      <c r="G49" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
         <v>1</v>
       </c>
-      <c r="E44" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.0)</f>
-        <v>13</v>
-      </c>
-      <c r="F44" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),44.0)</f>
-        <v>44</v>
-      </c>
-      <c r="G44" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),184.0)</f>
-        <v>184</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="5"/>
-    </row>
-    <row r="46">
-      <c r="C46" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D47" s="2">
+      <c r="H49" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="J49" s="13">
         <v>2.0</v>
       </c>
-      <c r="E47" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="F47" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="G47" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C48" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K48, ""      "")"),2.0)</f>
-        <v>2</v>
-      </c>
-      <c r="D48" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="E48" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
-      </c>
-      <c r="F48" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="G48" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
-        <v>3</v>
-      </c>
-      <c r="K48" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="13"/>
-      <c r="B49" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="C49" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K49, ""      "")"),10.0)</f>
-        <v>10</v>
-      </c>
-      <c r="D49" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.0)</f>
-        <v>4</v>
-      </c>
-      <c r="E49" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.0)</f>
-        <v>5</v>
-      </c>
-      <c r="F49" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
-        <v>6</v>
-      </c>
-      <c r="G49" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.0)</f>
-        <v>13</v>
-      </c>
-      <c r="K49" s="12" t="s">
-        <v>29</v>
+      <c r="K49" s="5" t="str">
+        <f t="shared" ref="K49:O49" si="28">ROUNDUP((C49/$M6), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L49" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>7.41%</v>
+      </c>
+      <c r="M49" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>77.78%</v>
+      </c>
+      <c r="N49" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>12.97%</v>
+      </c>
+      <c r="O49" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>1.86%</v>
       </c>
     </row>
     <row r="50">
@@ -2157,27 +2529,50 @@
         <v>3.0</v>
       </c>
       <c r="C50" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K50, ""      "")"),31.0)</f>
-        <v>31</v>
-      </c>
-      <c r="D50" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),42.0)</f>
-        <v>42</v>
-      </c>
-      <c r="E50" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H50, ""      "")"),2.0)</f>
+        <v>2</v>
+      </c>
+      <c r="D50" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),5.0)</f>
+        <v>5</v>
+      </c>
+      <c r="E50" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),69.0)</f>
         <v>69</v>
       </c>
-      <c r="F50" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),130.0)</f>
-        <v>130</v>
-      </c>
-      <c r="G50" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),387.0)</f>
-        <v>387</v>
-      </c>
-      <c r="K50" s="12" t="s">
-        <v>30</v>
+      <c r="F50" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),33.0)</f>
+        <v>33</v>
+      </c>
+      <c r="G50" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
+        <v>3</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J50" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="K50" s="5" t="str">
+        <f t="shared" ref="K50:O50" si="29">ROUNDUP((C50/$M7), 4)*100&amp;"%"</f>
+        <v>1.76%</v>
+      </c>
+      <c r="L50" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>4.39%</v>
+      </c>
+      <c r="M50" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>60.53%</v>
+      </c>
+      <c r="N50" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>28.95%</v>
+      </c>
+      <c r="O50" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>2.64%</v>
       </c>
     </row>
     <row r="51">
@@ -2186,27 +2581,50 @@
         <v>4.0</v>
       </c>
       <c r="C51" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K51, ""      "")"),7.0)</f>
-        <v>7</v>
-      </c>
-      <c r="D51" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
-        <v>7</v>
-      </c>
-      <c r="E51" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),33.0)</f>
-        <v>33</v>
-      </c>
-      <c r="F51" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H51, ""      "")"),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="D51" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
+        <v>6</v>
+      </c>
+      <c r="E51" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),130.0)</f>
+        <v>130</v>
+      </c>
+      <c r="F51" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),206.0)</f>
         <v>206</v>
       </c>
-      <c r="G51" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),733.0)</f>
-        <v>733</v>
-      </c>
-      <c r="K51" s="12" t="s">
-        <v>31</v>
+      <c r="G51" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),22.0)</f>
+        <v>22</v>
+      </c>
+      <c r="H51" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J51" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="K51" s="5" t="str">
+        <f t="shared" ref="K51:O51" si="30">ROUNDUP((C51/$M8), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L51" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>1.6%</v>
+      </c>
+      <c r="M51" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>34.67%</v>
+      </c>
+      <c r="N51" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>54.94%</v>
+      </c>
+      <c r="O51" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>5.87%</v>
       </c>
     </row>
     <row r="52">
@@ -2215,40 +2633,73 @@
         <v>5.0</v>
       </c>
       <c r="C52" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K52, ""      "")"),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="D52" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
-      </c>
-      <c r="E52" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H52, ""      "")"),3.0)</f>
         <v>3</v>
       </c>
-      <c r="F52" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),22.0)</f>
-        <v>22</v>
-      </c>
-      <c r="G52" s="11">
+      <c r="D52" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.0)</f>
+        <v>13</v>
+      </c>
+      <c r="E52" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),387.0)</f>
+        <v>387</v>
+      </c>
+      <c r="F52" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),733.0)</f>
+        <v>733</v>
+      </c>
+      <c r="G52" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),124.0)</f>
         <v>124</v>
       </c>
-      <c r="K52" s="12" t="s">
-        <v>32</v>
+      <c r="H52" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J52" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="K52" s="5" t="str">
+        <f t="shared" ref="K52:O52" si="31">ROUNDUP((C52/$M9), 4)*100&amp;"%"</f>
+        <v>0.24%</v>
+      </c>
+      <c r="L52" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>1.01%</v>
+      </c>
+      <c r="M52" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>29.89%</v>
+      </c>
+      <c r="N52" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>56.61%</v>
+      </c>
+      <c r="O52" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>9.58%</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="5"/>
     </row>
     <row r="54">
-      <c r="C54" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C54" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K54" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L54" s="12"/>
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+      <c r="O54" s="12"/>
     </row>
     <row r="55">
-      <c r="A55" s="10" t="s">
-        <v>16</v>
+      <c r="B55" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="C55" s="2">
         <v>1.0</v>
@@ -2265,65 +2716,126 @@
       <c r="G55" s="2">
         <v>5.0</v>
       </c>
+      <c r="J55" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K55" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="L55" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="M55" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="N55" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="O55" s="16">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="B56" s="2">
         <v>1.0</v>
       </c>
       <c r="C56" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K56, ""      "")"),0.0)</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H56, ""      "")"),0.0)</f>
         <v>0</v>
       </c>
-      <c r="D56" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
-      </c>
-      <c r="E56" s="11">
+      <c r="D56" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),8.0)</f>
+        <v>8</v>
+      </c>
+      <c r="E56" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),20.0)</f>
+        <v>20</v>
+      </c>
+      <c r="F56" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
+        <v>6</v>
+      </c>
+      <c r="G56" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
         <v>2</v>
       </c>
-      <c r="F56" s="11">
+      <c r="H56" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J56" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="K56" s="5" t="str">
+        <f t="shared" ref="K56:O56" si="32">ROUNDUP((C56/$N5), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L56" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>21.63%</v>
+      </c>
+      <c r="M56" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>54.06%</v>
+      </c>
+      <c r="N56" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>16.22%</v>
+      </c>
+      <c r="O56" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>5.41%</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="17"/>
+      <c r="B57" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="C57" s="8">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H57, ""      "")"),1.0)</f>
+        <v>1</v>
+      </c>
+      <c r="D57" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
+        <v>7</v>
+      </c>
+      <c r="E57" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),25.0)</f>
+        <v>25</v>
+      </c>
+      <c r="F57" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),11.0)</f>
+        <v>11</v>
+      </c>
+      <c r="G57" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
         <v>0</v>
       </c>
-      <c r="G56" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
-      </c>
-      <c r="K56" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="13"/>
-      <c r="B57" s="2">
+      <c r="H57" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J57" s="16">
         <v>2.0</v>
       </c>
-      <c r="C57" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K57, ""      "")"),8.0)</f>
-        <v>8</v>
-      </c>
-      <c r="D57" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
-        <v>7</v>
-      </c>
-      <c r="E57" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
-      </c>
-      <c r="F57" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
-        <v>3</v>
-      </c>
-      <c r="G57" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.0)</f>
-        <v>10</v>
-      </c>
-      <c r="K57" s="12" t="s">
-        <v>34</v>
+      <c r="K57" s="5" t="str">
+        <f t="shared" ref="K57:O57" si="33">ROUNDUP((C57/$N6), 4)*100&amp;"%"</f>
+        <v>2.18%</v>
+      </c>
+      <c r="L57" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>15.22%</v>
+      </c>
+      <c r="M57" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>54.35%</v>
+      </c>
+      <c r="N57" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>23.92%</v>
+      </c>
+      <c r="O57" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>0%</v>
       </c>
     </row>
     <row r="58">
@@ -2332,27 +2844,50 @@
         <v>3.0</v>
       </c>
       <c r="C58" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K58, ""      "")"),20.0)</f>
-        <v>20</v>
-      </c>
-      <c r="D58" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),25.0)</f>
-        <v>25</v>
-      </c>
-      <c r="E58" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H58, ""      "")"),2.0)</f>
+        <v>2</v>
+      </c>
+      <c r="D58" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
+        <v>2</v>
+      </c>
+      <c r="E58" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),72.0)</f>
         <v>72</v>
       </c>
-      <c r="F58" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),161.0)</f>
-        <v>161</v>
-      </c>
-      <c r="G58" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),371.0)</f>
-        <v>371</v>
-      </c>
-      <c r="K58" s="12" t="s">
-        <v>35</v>
+      <c r="F58" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),40.0)</f>
+        <v>40</v>
+      </c>
+      <c r="G58" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.0)</f>
+        <v>4</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J58" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="K58" s="5" t="str">
+        <f t="shared" ref="K58:O58" si="34">ROUNDUP((C58/$N7), 4)*100&amp;"%"</f>
+        <v>1.59%</v>
+      </c>
+      <c r="L58" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>1.59%</v>
+      </c>
+      <c r="M58" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>57.15%</v>
+      </c>
+      <c r="N58" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>31.75%</v>
+      </c>
+      <c r="O58" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>3.18%</v>
       </c>
     </row>
     <row r="59">
@@ -2361,27 +2896,50 @@
         <v>4.0</v>
       </c>
       <c r="C59" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K59, ""      "")"),6.0)</f>
-        <v>6</v>
-      </c>
-      <c r="D59" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),11.0)</f>
-        <v>11</v>
-      </c>
-      <c r="E59" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),40.0)</f>
-        <v>40</v>
-      </c>
-      <c r="F59" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H59, ""      "")"),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="D59" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
+        <v>3</v>
+      </c>
+      <c r="E59" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),161.0)</f>
+        <v>161</v>
+      </c>
+      <c r="F59" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),239.0)</f>
         <v>239</v>
       </c>
-      <c r="G59" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),738.0)</f>
-        <v>738</v>
-      </c>
-      <c r="K59" s="12" t="s">
-        <v>36</v>
+      <c r="G59" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),23.0)</f>
+        <v>23</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J59" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="K59" s="5" t="str">
+        <f t="shared" ref="K59:O59" si="35">ROUNDUP((C59/$N8), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L59" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>0.7%</v>
+      </c>
+      <c r="M59" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>37.1%</v>
+      </c>
+      <c r="N59" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>55.07%</v>
+      </c>
+      <c r="O59" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>5.3%</v>
       </c>
     </row>
     <row r="60">
@@ -2390,40 +2948,73 @@
         <v>5.0</v>
       </c>
       <c r="C60" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K60, ""      "")"),2.0)</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H60, ""      "")"),2.0)</f>
         <v>2</v>
       </c>
-      <c r="D60" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="E60" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.0)</f>
-        <v>4</v>
-      </c>
-      <c r="F60" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),23.0)</f>
-        <v>23</v>
-      </c>
-      <c r="G60" s="11">
+      <c r="D60" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.0)</f>
+        <v>10</v>
+      </c>
+      <c r="E60" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),371.0)</f>
+        <v>371</v>
+      </c>
+      <c r="F60" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),738.0)</f>
+        <v>738</v>
+      </c>
+      <c r="G60" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),124.0)</f>
         <v>124</v>
       </c>
-      <c r="K60" s="12" t="s">
-        <v>37</v>
+      <c r="H60" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J60" s="16">
+        <v>5.0</v>
+      </c>
+      <c r="K60" s="5" t="str">
+        <f t="shared" ref="K60:O60" si="36">ROUNDUP((C60/$N9), 4)*100&amp;"%"</f>
+        <v>0.16%</v>
+      </c>
+      <c r="L60" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>0.79%</v>
+      </c>
+      <c r="M60" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>29.08%</v>
+      </c>
+      <c r="N60" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>57.84%</v>
+      </c>
+      <c r="O60" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>9.72%</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="5"/>
     </row>
     <row r="62">
-      <c r="C62" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C62" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K62" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L62" s="12"/>
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="12"/>
     </row>
     <row r="63">
-      <c r="A63" s="10" t="s">
-        <v>16</v>
+      <c r="B63" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="C63" s="2">
         <v>1.0</v>
@@ -2440,65 +3031,126 @@
       <c r="G63" s="2">
         <v>5.0</v>
       </c>
+      <c r="J63" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K63" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="L63" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="M63" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="N63" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="O63" s="16">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="B64" s="2">
         <v>1.0</v>
       </c>
       <c r="C64" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K64, ""      "")"),7.0)</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H64, ""      "")"),7.0)</f>
         <v>7</v>
       </c>
-      <c r="D64" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
-      </c>
-      <c r="E64" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
-        <v>7</v>
-      </c>
-      <c r="F64" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
-        <v>7</v>
-      </c>
-      <c r="G64" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),8.0)</f>
-        <v>8</v>
-      </c>
-      <c r="K64" s="12" t="s">
-        <v>38</v>
+      <c r="D64" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),46.0)</f>
+        <v>46</v>
+      </c>
+      <c r="E64" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),149.0)</f>
+        <v>149</v>
+      </c>
+      <c r="F64" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),30.0)</f>
+        <v>30</v>
+      </c>
+      <c r="G64" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
+        <v>3</v>
+      </c>
+      <c r="H64" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J64" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="K64" s="5" t="str">
+        <f t="shared" ref="K64:O64" si="37">ROUNDUP((C64/$O5), 4)*100&amp;"%"</f>
+        <v>2.91%</v>
+      </c>
+      <c r="L64" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>19.09%</v>
+      </c>
+      <c r="M64" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>61.83%</v>
+      </c>
+      <c r="N64" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>12.45%</v>
+      </c>
+      <c r="O64" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>1.25%</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="13"/>
+      <c r="A65" s="17"/>
       <c r="B65" s="2">
         <v>2.0</v>
       </c>
       <c r="C65" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K65, ""      "")"),46.0)</f>
-        <v>46</v>
-      </c>
-      <c r="D65" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H65, ""      "")"),1.0)</f>
+        <v>1</v>
+      </c>
+      <c r="D65" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),29.0)</f>
         <v>29</v>
       </c>
-      <c r="E65" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),36.0)</f>
-        <v>36</v>
-      </c>
-      <c r="F65" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),38.0)</f>
-        <v>38</v>
-      </c>
-      <c r="G65" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),74.0)</f>
-        <v>74</v>
-      </c>
-      <c r="K65" s="12" t="s">
-        <v>39</v>
+      <c r="E65" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),138.0)</f>
+        <v>138</v>
+      </c>
+      <c r="F65" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),32.0)</f>
+        <v>32</v>
+      </c>
+      <c r="G65" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
+        <v>3</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J65" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="K65" s="5" t="str">
+        <f t="shared" ref="K65:O65" si="38">ROUNDUP((C65/$O6), 4)*100&amp;"%"</f>
+        <v>0.49%</v>
+      </c>
+      <c r="L65" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>14.08%</v>
+      </c>
+      <c r="M65" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>67%</v>
+      </c>
+      <c r="N65" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>15.54%</v>
+      </c>
+      <c r="O65" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>1.46%</v>
       </c>
     </row>
     <row r="66">
@@ -2507,27 +3159,50 @@
         <v>3.0</v>
       </c>
       <c r="C66" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K66, ""      "")"),149.0)</f>
-        <v>149</v>
-      </c>
-      <c r="D66" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),138.0)</f>
-        <v>138</v>
-      </c>
-      <c r="E66" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H66, ""      "")"),7.0)</f>
+        <v>7</v>
+      </c>
+      <c r="D66" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),36.0)</f>
+        <v>36</v>
+      </c>
+      <c r="E66" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),227.0)</f>
         <v>227</v>
       </c>
-      <c r="F66" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),325.0)</f>
-        <v>325</v>
-      </c>
-      <c r="G66" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),751.0)</f>
-        <v>751</v>
-      </c>
-      <c r="K66" s="12" t="s">
-        <v>40</v>
+      <c r="F66" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),120.0)</f>
+        <v>120</v>
+      </c>
+      <c r="G66" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),21.0)</f>
+        <v>21</v>
+      </c>
+      <c r="H66" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J66" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="K66" s="5" t="str">
+        <f t="shared" ref="K66:O66" si="39">ROUNDUP((C66/$O7), 4)*100&amp;"%"</f>
+        <v>1.66%</v>
+      </c>
+      <c r="L66" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>8.54%</v>
+      </c>
+      <c r="M66" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>53.8%</v>
+      </c>
+      <c r="N66" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>28.44%</v>
+      </c>
+      <c r="O66" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>4.98%</v>
       </c>
     </row>
     <row r="67">
@@ -2536,27 +3211,50 @@
         <v>4.0</v>
       </c>
       <c r="C67" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K67, ""      "")"),30.0)</f>
-        <v>30</v>
-      </c>
-      <c r="D67" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),32.0)</f>
-        <v>32</v>
-      </c>
-      <c r="E67" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),120.0)</f>
-        <v>120</v>
-      </c>
-      <c r="F67" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H67, ""      "")"),7.0)</f>
+        <v>7</v>
+      </c>
+      <c r="D67" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),38.0)</f>
+        <v>38</v>
+      </c>
+      <c r="E67" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),325.0)</f>
+        <v>325</v>
+      </c>
+      <c r="F67" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),329.0)</f>
         <v>329</v>
       </c>
-      <c r="G67" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1225.0)</f>
-        <v>1225</v>
-      </c>
-      <c r="K67" s="12" t="s">
-        <v>41</v>
+      <c r="G67" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),79.0)</f>
+        <v>79</v>
+      </c>
+      <c r="H67" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J67" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="K67" s="5" t="str">
+        <f t="shared" ref="K67:O67" si="40">ROUNDUP((C67/$O8), 4)*100&amp;"%"</f>
+        <v>0.89%</v>
+      </c>
+      <c r="L67" s="5" t="str">
+        <f t="shared" si="40"/>
+        <v>4.83%</v>
+      </c>
+      <c r="M67" s="5" t="str">
+        <f t="shared" si="40"/>
+        <v>41.25%</v>
+      </c>
+      <c r="N67" s="5" t="str">
+        <f t="shared" si="40"/>
+        <v>41.76%</v>
+      </c>
+      <c r="O67" s="5" t="str">
+        <f t="shared" si="40"/>
+        <v>10.03%</v>
       </c>
     </row>
     <row r="68">
@@ -2565,40 +3263,73 @@
         <v>5.0</v>
       </c>
       <c r="C68" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K68, ""      "")"),3.0)</f>
-        <v>3</v>
-      </c>
-      <c r="D68" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
-        <v>3</v>
-      </c>
-      <c r="E68" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),21.0)</f>
-        <v>21</v>
-      </c>
-      <c r="F68" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),79.0)</f>
-        <v>79</v>
-      </c>
-      <c r="G68" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H68, ""      "")"),8.0)</f>
+        <v>8</v>
+      </c>
+      <c r="D68" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),74.0)</f>
+        <v>74</v>
+      </c>
+      <c r="E68" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),751.0)</f>
+        <v>751</v>
+      </c>
+      <c r="F68" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1225.0)</f>
+        <v>1225</v>
+      </c>
+      <c r="G68" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),342.0)</f>
         <v>342</v>
       </c>
-      <c r="K68" s="12" t="s">
-        <v>42</v>
+      <c r="H68" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J68" s="16">
+        <v>5.0</v>
+      </c>
+      <c r="K68" s="5" t="str">
+        <f t="shared" ref="K68:O68" si="41">ROUNDUP((C68/$O9), 4)*100&amp;"%"</f>
+        <v>0.33%</v>
+      </c>
+      <c r="L68" s="5" t="str">
+        <f t="shared" si="41"/>
+        <v>3.01%</v>
+      </c>
+      <c r="M68" s="5" t="str">
+        <f t="shared" si="41"/>
+        <v>30.48%</v>
+      </c>
+      <c r="N68" s="5" t="str">
+        <f t="shared" si="41"/>
+        <v>49.72%</v>
+      </c>
+      <c r="O68" s="5" t="str">
+        <f t="shared" si="41"/>
+        <v>13.88%</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="5"/>
     </row>
     <row r="70">
-      <c r="C70" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C70" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K70" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L70" s="12"/>
+      <c r="M70" s="12"/>
+      <c r="N70" s="12"/>
+      <c r="O70" s="12"/>
     </row>
     <row r="71">
-      <c r="A71" s="10" t="s">
-        <v>16</v>
+      <c r="B71" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="C71" s="2">
         <v>1.0</v>
@@ -2615,65 +3346,126 @@
       <c r="G71" s="2">
         <v>5.0</v>
       </c>
+      <c r="J71" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K71" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="L71" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="M71" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="N71" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="O71" s="16">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="72">
-      <c r="A72" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="B72" s="2">
         <v>1.0</v>
       </c>
       <c r="C72" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K72, ""      "")"),0.0)</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H72, ""      "")"),0.0)</f>
         <v>0</v>
       </c>
-      <c r="D72" s="11">
+      <c r="D72" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),15.0)</f>
+        <v>15</v>
+      </c>
+      <c r="E72" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),128.0)</f>
+        <v>128</v>
+      </c>
+      <c r="F72" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),12.0)</f>
+        <v>12</v>
+      </c>
+      <c r="G72" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.0)</f>
+        <v>4</v>
+      </c>
+      <c r="H72" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="J72" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="K72" s="5" t="str">
+        <f t="shared" ref="K72:O72" si="42">ROUNDUP((C72/$P5), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L72" s="5" t="str">
+        <f t="shared" si="42"/>
+        <v>9.1%</v>
+      </c>
+      <c r="M72" s="5" t="str">
+        <f t="shared" si="42"/>
+        <v>77.58%</v>
+      </c>
+      <c r="N72" s="5" t="str">
+        <f t="shared" si="42"/>
+        <v>7.28%</v>
+      </c>
+      <c r="O72" s="5" t="str">
+        <f t="shared" si="42"/>
+        <v>2.43%</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="17"/>
+      <c r="B73" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="C73" s="8">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H73, ""      "")"),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="D73" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.0)</f>
+        <v>10</v>
+      </c>
+      <c r="E73" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),71.0)</f>
+        <v>71</v>
+      </c>
+      <c r="F73" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.0)</f>
+        <v>13</v>
+      </c>
+      <c r="G73" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
         <v>0</v>
       </c>
-      <c r="E72" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="F72" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="G72" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="K72" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="13"/>
-      <c r="B73" s="2">
+      <c r="H73" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J73" s="16">
         <v>2.0</v>
       </c>
-      <c r="C73" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K73, ""      "")"),15.0)</f>
-        <v>15</v>
-      </c>
-      <c r="D73" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.0)</f>
-        <v>10</v>
-      </c>
-      <c r="E73" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
-        <v>6</v>
-      </c>
-      <c r="F73" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),9.0)</f>
-        <v>9</v>
-      </c>
-      <c r="G73" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),12.0)</f>
-        <v>12</v>
-      </c>
-      <c r="K73" s="12" t="s">
-        <v>44</v>
+      <c r="K73" s="5" t="str">
+        <f t="shared" ref="K73:O73" si="43">ROUNDUP((C73/$P6), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L73" s="5" t="str">
+        <f t="shared" si="43"/>
+        <v>10.42%</v>
+      </c>
+      <c r="M73" s="5" t="str">
+        <f t="shared" si="43"/>
+        <v>73.96%</v>
+      </c>
+      <c r="N73" s="5" t="str">
+        <f t="shared" si="43"/>
+        <v>13.55%</v>
+      </c>
+      <c r="O73" s="5" t="str">
+        <f t="shared" si="43"/>
+        <v>0%</v>
       </c>
     </row>
     <row r="74">
@@ -2682,27 +3474,50 @@
         <v>3.0</v>
       </c>
       <c r="C74" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K74, ""      "")"),128.0)</f>
-        <v>128</v>
-      </c>
-      <c r="D74" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),71.0)</f>
-        <v>71</v>
-      </c>
-      <c r="E74" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H74, ""      "")"),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="D74" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
+        <v>6</v>
+      </c>
+      <c r="E74" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),110.0)</f>
         <v>110</v>
       </c>
-      <c r="F74" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),166.0)</f>
-        <v>166</v>
-      </c>
-      <c r="G74" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),432.0)</f>
-        <v>432</v>
-      </c>
-      <c r="K74" s="12" t="s">
-        <v>45</v>
+      <c r="F74" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),48.0)</f>
+        <v>48</v>
+      </c>
+      <c r="G74" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
+        <v>3</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J74" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="K74" s="5" t="str">
+        <f t="shared" ref="K74:O74" si="44">ROUNDUP((C74/$P7), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L74" s="5" t="str">
+        <f t="shared" si="44"/>
+        <v>3.51%</v>
+      </c>
+      <c r="M74" s="5" t="str">
+        <f t="shared" si="44"/>
+        <v>64.33%</v>
+      </c>
+      <c r="N74" s="5" t="str">
+        <f t="shared" si="44"/>
+        <v>28.08%</v>
+      </c>
+      <c r="O74" s="5" t="str">
+        <f t="shared" si="44"/>
+        <v>1.76%</v>
       </c>
     </row>
     <row r="75">
@@ -2711,27 +3526,50 @@
         <v>4.0</v>
       </c>
       <c r="C75" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K75, ""      "")"),12.0)</f>
-        <v>12</v>
-      </c>
-      <c r="D75" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.0)</f>
-        <v>13</v>
-      </c>
-      <c r="E75" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),48.0)</f>
-        <v>48</v>
-      </c>
-      <c r="F75" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H75, ""      "")"),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="D75" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),9.0)</f>
+        <v>9</v>
+      </c>
+      <c r="E75" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),166.0)</f>
+        <v>166</v>
+      </c>
+      <c r="F75" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),182.0)</f>
         <v>182</v>
       </c>
-      <c r="G75" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),711.0)</f>
-        <v>711</v>
-      </c>
-      <c r="K75" s="12" t="s">
-        <v>46</v>
+      <c r="G75" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),23.0)</f>
+        <v>23</v>
+      </c>
+      <c r="H75" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J75" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="K75" s="5" t="str">
+        <f t="shared" ref="K75:O75" si="45">ROUNDUP((C75/$P8), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L75" s="5" t="str">
+        <f t="shared" si="45"/>
+        <v>2.33%</v>
+      </c>
+      <c r="M75" s="5" t="str">
+        <f t="shared" si="45"/>
+        <v>42.9%</v>
+      </c>
+      <c r="N75" s="5" t="str">
+        <f t="shared" si="45"/>
+        <v>47.03%</v>
+      </c>
+      <c r="O75" s="5" t="str">
+        <f t="shared" si="45"/>
+        <v>5.95%</v>
       </c>
     </row>
     <row r="76">
@@ -2740,40 +3578,73 @@
         <v>5.0</v>
       </c>
       <c r="C76" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K76, ""      "")"),4.0)</f>
-        <v>4</v>
-      </c>
-      <c r="D76" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H76, ""      "")"),0.0)</f>
         <v>0</v>
       </c>
-      <c r="E76" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
-        <v>3</v>
-      </c>
-      <c r="F76" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),23.0)</f>
-        <v>23</v>
-      </c>
-      <c r="G76" s="11">
+      <c r="D76" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),12.0)</f>
+        <v>12</v>
+      </c>
+      <c r="E76" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),432.0)</f>
+        <v>432</v>
+      </c>
+      <c r="F76" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),711.0)</f>
+        <v>711</v>
+      </c>
+      <c r="G76" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),132.0)</f>
         <v>132</v>
       </c>
-      <c r="K76" s="12" t="s">
-        <v>47</v>
+      <c r="H76" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J76" s="16">
+        <v>5.0</v>
+      </c>
+      <c r="K76" s="5" t="str">
+        <f t="shared" ref="K76:O76" si="46">ROUNDUP((C76/$P9), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L76" s="5" t="str">
+        <f t="shared" si="46"/>
+        <v>0.91%</v>
+      </c>
+      <c r="M76" s="5" t="str">
+        <f t="shared" si="46"/>
+        <v>32.63%</v>
+      </c>
+      <c r="N76" s="5" t="str">
+        <f t="shared" si="46"/>
+        <v>53.71%</v>
+      </c>
+      <c r="O76" s="5" t="str">
+        <f t="shared" si="46"/>
+        <v>9.97%</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="5"/>
     </row>
     <row r="78">
-      <c r="C78" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C78" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K78" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L78" s="12"/>
+      <c r="M78" s="12"/>
+      <c r="N78" s="12"/>
+      <c r="O78" s="12"/>
     </row>
     <row r="79">
-      <c r="A79" s="10" t="s">
-        <v>16</v>
+      <c r="B79" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="C79" s="2">
         <v>1.0</v>
@@ -2790,65 +3661,126 @@
       <c r="G79" s="2">
         <v>5.0</v>
       </c>
+      <c r="J79" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K79" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="L79" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="M79" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="N79" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="O79" s="13">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="80">
-      <c r="A80" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="B80" s="2">
         <v>1.0</v>
       </c>
       <c r="C80" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K80, ""      "")"),0.0)</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H80, ""      "")"),0.0)</f>
         <v>0</v>
       </c>
-      <c r="D80" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
-      </c>
-      <c r="E80" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="F80" s="11">
+      <c r="D80" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),8.0)</f>
+        <v>8</v>
+      </c>
+      <c r="E80" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),43.0)</f>
+        <v>43</v>
+      </c>
+      <c r="F80" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),8.0)</f>
+        <v>8</v>
+      </c>
+      <c r="G80" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
         <v>1</v>
       </c>
-      <c r="G80" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="K80" s="12" t="s">
-        <v>48</v>
+      <c r="H80" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J80" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="K80" s="5" t="str">
+        <f t="shared" ref="K80:O80" si="47">ROUNDUP((C80/$Q5), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L80" s="5" t="str">
+        <f t="shared" si="47"/>
+        <v>12.91%</v>
+      </c>
+      <c r="M80" s="5" t="str">
+        <f t="shared" si="47"/>
+        <v>69.36%</v>
+      </c>
+      <c r="N80" s="5" t="str">
+        <f t="shared" si="47"/>
+        <v>12.91%</v>
+      </c>
+      <c r="O80" s="5" t="str">
+        <f t="shared" si="47"/>
+        <v>1.62%</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="13"/>
+      <c r="A81" s="17"/>
       <c r="B81" s="2">
         <v>2.0</v>
       </c>
       <c r="C81" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K81, ""      "")"),8.0)</f>
-        <v>8</v>
-      </c>
-      <c r="D81" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H81, ""      "")"),2.0)</f>
+        <v>2</v>
+      </c>
+      <c r="D81" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),12.0)</f>
         <v>12</v>
       </c>
-      <c r="E81" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
-        <v>7</v>
-      </c>
-      <c r="F81" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
-        <v>7</v>
-      </c>
-      <c r="G81" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
-      </c>
-      <c r="K81" s="12" t="s">
-        <v>49</v>
+      <c r="E81" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),63.0)</f>
+        <v>63</v>
+      </c>
+      <c r="F81" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),22.0)</f>
+        <v>22</v>
+      </c>
+      <c r="G81" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
+      </c>
+      <c r="H81" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J81" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="K81" s="5" t="str">
+        <f t="shared" ref="K81:O81" si="48">ROUNDUP((C81/$Q6), 4)*100&amp;"%"</f>
+        <v>2%</v>
+      </c>
+      <c r="L81" s="5" t="str">
+        <f t="shared" si="48"/>
+        <v>12%</v>
+      </c>
+      <c r="M81" s="5" t="str">
+        <f t="shared" si="48"/>
+        <v>63%</v>
+      </c>
+      <c r="N81" s="5" t="str">
+        <f t="shared" si="48"/>
+        <v>22%</v>
+      </c>
+      <c r="O81" s="5" t="str">
+        <f t="shared" si="48"/>
+        <v>1%</v>
       </c>
     </row>
     <row r="82">
@@ -2857,27 +3789,50 @@
         <v>3.0</v>
       </c>
       <c r="C82" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K82, ""      "")"),43.0)</f>
-        <v>43</v>
-      </c>
-      <c r="D82" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),63.0)</f>
-        <v>63</v>
-      </c>
-      <c r="E82" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H82, ""      "")"),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="D82" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
+        <v>7</v>
+      </c>
+      <c r="E82" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),82.0)</f>
         <v>82</v>
       </c>
-      <c r="F82" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),118.0)</f>
-        <v>118</v>
-      </c>
-      <c r="G82" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),245.0)</f>
-        <v>245</v>
-      </c>
-      <c r="K82" s="12" t="s">
-        <v>50</v>
+      <c r="F82" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),70.0)</f>
+        <v>70</v>
+      </c>
+      <c r="G82" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
+        <v>6</v>
+      </c>
+      <c r="H82" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J82" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="K82" s="5" t="str">
+        <f t="shared" ref="K82:O82" si="49">ROUNDUP((C82/$Q7), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L82" s="5" t="str">
+        <f t="shared" si="49"/>
+        <v>4.12%</v>
+      </c>
+      <c r="M82" s="5" t="str">
+        <f t="shared" si="49"/>
+        <v>48.24%</v>
+      </c>
+      <c r="N82" s="5" t="str">
+        <f t="shared" si="49"/>
+        <v>41.18%</v>
+      </c>
+      <c r="O82" s="5" t="str">
+        <f t="shared" si="49"/>
+        <v>3.53%</v>
       </c>
     </row>
     <row r="83">
@@ -2886,27 +3841,50 @@
         <v>4.0</v>
       </c>
       <c r="C83" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K83, ""      "")"),8.0)</f>
-        <v>8</v>
-      </c>
-      <c r="D83" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),22.0)</f>
-        <v>22</v>
-      </c>
-      <c r="E83" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),70.0)</f>
-        <v>70</v>
-      </c>
-      <c r="F83" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H83, ""      "")"),1.0)</f>
+        <v>1</v>
+      </c>
+      <c r="D83" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),7.0)</f>
+        <v>7</v>
+      </c>
+      <c r="E83" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),118.0)</f>
+        <v>118</v>
+      </c>
+      <c r="F83" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),192.0)</f>
         <v>192</v>
       </c>
-      <c r="G83" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),751.0)</f>
-        <v>751</v>
-      </c>
-      <c r="K83" s="12" t="s">
-        <v>51</v>
+      <c r="G83" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),38.0)</f>
+        <v>38</v>
+      </c>
+      <c r="H83" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J83" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="K83" s="5" t="str">
+        <f t="shared" ref="K83:O83" si="50">ROUNDUP((C83/$Q8), 4)*100&amp;"%"</f>
+        <v>0.28%</v>
+      </c>
+      <c r="L83" s="5" t="str">
+        <f t="shared" si="50"/>
+        <v>1.94%</v>
+      </c>
+      <c r="M83" s="5" t="str">
+        <f t="shared" si="50"/>
+        <v>32.69%</v>
+      </c>
+      <c r="N83" s="5" t="str">
+        <f t="shared" si="50"/>
+        <v>53.19%</v>
+      </c>
+      <c r="O83" s="5" t="str">
+        <f t="shared" si="50"/>
+        <v>10.53%</v>
       </c>
     </row>
     <row r="84">
@@ -2915,115 +3893,209 @@
         <v>5.0</v>
       </c>
       <c r="C84" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K84, ""      "")"),1.0)</f>
-        <v>1</v>
-      </c>
-      <c r="D84" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H84, ""      "")"),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="D84" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
+        <v>2</v>
+      </c>
+      <c r="E84" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),245.0)</f>
+        <v>245</v>
+      </c>
+      <c r="F84" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),751.0)</f>
+        <v>751</v>
+      </c>
+      <c r="G84" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),229.0)</f>
+        <v>229</v>
+      </c>
+      <c r="H84" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J84" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="K84" s="5" t="str">
+        <f t="shared" ref="K84:O84" si="51">ROUNDUP((C84/$Q9), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L84" s="5" t="str">
+        <f t="shared" si="51"/>
+        <v>0.16%</v>
+      </c>
+      <c r="M84" s="5" t="str">
+        <f t="shared" si="51"/>
+        <v>19.42%</v>
+      </c>
+      <c r="N84" s="5" t="str">
+        <f t="shared" si="51"/>
+        <v>59.51%</v>
+      </c>
+      <c r="O84" s="5" t="str">
+        <f t="shared" si="51"/>
+        <v>18.15%</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="5"/>
+    </row>
+    <row r="86">
+      <c r="B86" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K86" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L86" s="12"/>
+      <c r="M86" s="12"/>
+      <c r="N86" s="12"/>
+      <c r="O86" s="12"/>
+    </row>
+    <row r="87">
+      <c r="B87" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D87" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E87" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F87" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="G87" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="J87" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K87" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="L87" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="M87" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="N87" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="O87" s="13">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C88" s="8">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H88, ""      "")"),2.0)</f>
+        <v>2</v>
+      </c>
+      <c r="D88" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),18.0)</f>
+        <v>18</v>
+      </c>
+      <c r="E88" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),77.0)</f>
+        <v>77</v>
+      </c>
+      <c r="F88" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.0)</f>
+        <v>10</v>
+      </c>
+      <c r="G88" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
         <v>1</v>
       </c>
-      <c r="E84" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
-        <v>6</v>
-      </c>
-      <c r="F84" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),38.0)</f>
-        <v>38</v>
-      </c>
-      <c r="G84" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),229.0)</f>
-        <v>229</v>
-      </c>
-      <c r="K84" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="5"/>
-    </row>
-    <row r="86">
-      <c r="C86" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="10" t="s">
+      <c r="H88" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J88" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="K88" s="5" t="str">
+        <f t="shared" ref="K88:O88" si="52">ROUNDUP((C88/$R5), 4)*100&amp;"%"</f>
+        <v>1.82%</v>
+      </c>
+      <c r="L88" s="5" t="str">
+        <f t="shared" si="52"/>
+        <v>16.37%</v>
+      </c>
+      <c r="M88" s="5" t="str">
+        <f t="shared" si="52"/>
+        <v>70%</v>
+      </c>
+      <c r="N88" s="5" t="str">
+        <f t="shared" si="52"/>
+        <v>9.1%</v>
+      </c>
+      <c r="O88" s="5" t="str">
+        <f t="shared" si="52"/>
+        <v>0.91%</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="17"/>
+      <c r="B89" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="C89" s="8">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H89, ""      "")"),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="D89" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),19.0)</f>
+        <v>19</v>
+      </c>
+      <c r="E89" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),83.0)</f>
+        <v>83</v>
+      </c>
+      <c r="F89" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),16.0)</f>
         <v>16</v>
       </c>
-      <c r="C87" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D87" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="E87" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="F87" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="G87" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B88" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C88" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K88, ""      "")"),2.0)</f>
-        <v>2</v>
-      </c>
-      <c r="D88" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="E88" s="11">
+      <c r="G89" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
         <v>2</v>
       </c>
-      <c r="F88" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="G88" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="K88" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="13"/>
-      <c r="B89" s="2">
+      <c r="H89" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="J89" s="16">
         <v>2.0</v>
       </c>
-      <c r="C89" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K89, ""      "")"),18.0)</f>
-        <v>18</v>
-      </c>
-      <c r="D89" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),19.0)</f>
-        <v>19</v>
-      </c>
-      <c r="E89" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
-        <v>6</v>
-      </c>
-      <c r="F89" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
-        <v>3</v>
-      </c>
-      <c r="G89" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),11.0)</f>
-        <v>11</v>
-      </c>
-      <c r="K89" s="12" t="s">
-        <v>54</v>
+      <c r="K89" s="5" t="str">
+        <f t="shared" ref="K89:O89" si="53">ROUNDUP((C89/$R6), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L89" s="5" t="str">
+        <f t="shared" si="53"/>
+        <v>15.58%</v>
+      </c>
+      <c r="M89" s="5" t="str">
+        <f t="shared" si="53"/>
+        <v>68.04%</v>
+      </c>
+      <c r="N89" s="5" t="str">
+        <f t="shared" si="53"/>
+        <v>13.12%</v>
+      </c>
+      <c r="O89" s="5" t="str">
+        <f t="shared" si="53"/>
+        <v>1.64%</v>
       </c>
     </row>
     <row r="90">
@@ -3032,27 +4104,50 @@
         <v>3.0</v>
       </c>
       <c r="C90" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K90, ""      "")"),77.0)</f>
-        <v>77</v>
-      </c>
-      <c r="D90" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),83.0)</f>
-        <v>83</v>
-      </c>
-      <c r="E90" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H90, ""      "")"),2.0)</f>
+        <v>2</v>
+      </c>
+      <c r="D90" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
+        <v>6</v>
+      </c>
+      <c r="E90" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),114.0)</f>
         <v>114</v>
       </c>
-      <c r="F90" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),109.0)</f>
-        <v>109</v>
-      </c>
-      <c r="G90" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),308.0)</f>
-        <v>308</v>
-      </c>
-      <c r="K90" s="12" t="s">
-        <v>55</v>
+      <c r="F90" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),62.0)</f>
+        <v>62</v>
+      </c>
+      <c r="G90" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),15.0)</f>
+        <v>15</v>
+      </c>
+      <c r="H90" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J90" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="K90" s="5" t="str">
+        <f t="shared" ref="K90:O90" si="54">ROUNDUP((C90/$R7), 4)*100&amp;"%"</f>
+        <v>0.99%</v>
+      </c>
+      <c r="L90" s="5" t="str">
+        <f t="shared" si="54"/>
+        <v>2.96%</v>
+      </c>
+      <c r="M90" s="5" t="str">
+        <f t="shared" si="54"/>
+        <v>56.16%</v>
+      </c>
+      <c r="N90" s="5" t="str">
+        <f t="shared" si="54"/>
+        <v>30.55%</v>
+      </c>
+      <c r="O90" s="5" t="str">
+        <f t="shared" si="54"/>
+        <v>7.39%</v>
       </c>
     </row>
     <row r="91">
@@ -3061,27 +4156,50 @@
         <v>4.0</v>
       </c>
       <c r="C91" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K91, ""      "")"),10.0)</f>
-        <v>10</v>
-      </c>
-      <c r="D91" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),16.0)</f>
-        <v>16</v>
-      </c>
-      <c r="E91" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),62.0)</f>
-        <v>62</v>
-      </c>
-      <c r="F91" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H91, ""      "")"),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="D91" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
+        <v>3</v>
+      </c>
+      <c r="E91" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),109.0)</f>
+        <v>109</v>
+      </c>
+      <c r="F91" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),168.0)</f>
         <v>168</v>
       </c>
-      <c r="G91" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),606.0)</f>
-        <v>606</v>
-      </c>
-      <c r="K91" s="12" t="s">
-        <v>56</v>
+      <c r="G91" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),25.0)</f>
+        <v>25</v>
+      </c>
+      <c r="H91" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J91" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="K91" s="5" t="str">
+        <f t="shared" ref="K91:O91" si="55">ROUNDUP((C91/$R8), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L91" s="5" t="str">
+        <f t="shared" si="55"/>
+        <v>0.97%</v>
+      </c>
+      <c r="M91" s="5" t="str">
+        <f t="shared" si="55"/>
+        <v>35.05%</v>
+      </c>
+      <c r="N91" s="5" t="str">
+        <f t="shared" si="55"/>
+        <v>54.02%</v>
+      </c>
+      <c r="O91" s="5" t="str">
+        <f t="shared" si="55"/>
+        <v>8.04%</v>
       </c>
     </row>
     <row r="92">
@@ -3090,27 +4208,50 @@
         <v>5.0</v>
       </c>
       <c r="C92" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(K92, ""      "")"),1.0)</f>
-        <v>1</v>
-      </c>
-      <c r="D92" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
-      </c>
-      <c r="E92" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),15.0)</f>
-        <v>15</v>
-      </c>
-      <c r="F92" s="11">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),25.0)</f>
-        <v>25</v>
-      </c>
-      <c r="G92" s="11">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(H92, ""      "")"),0.0)</f>
+        <v>0</v>
+      </c>
+      <c r="D92" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),11.0)</f>
+        <v>11</v>
+      </c>
+      <c r="E92" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),308.0)</f>
+        <v>308</v>
+      </c>
+      <c r="F92" s="14">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),606.0)</f>
+        <v>606</v>
+      </c>
+      <c r="G92" s="14">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),100.0)</f>
         <v>100</v>
       </c>
-      <c r="K92" s="12" t="s">
-        <v>57</v>
+      <c r="H92" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J92" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="K92" s="5" t="str">
+        <f t="shared" ref="K92:O92" si="56">ROUNDUP((C92/$R9), 4)*100&amp;"%"</f>
+        <v>0%</v>
+      </c>
+      <c r="L92" s="5" t="str">
+        <f t="shared" si="56"/>
+        <v>1.06%</v>
+      </c>
+      <c r="M92" s="5" t="str">
+        <f t="shared" si="56"/>
+        <v>29.51%</v>
+      </c>
+      <c r="N92" s="5" t="str">
+        <f t="shared" si="56"/>
+        <v>58.05%</v>
+      </c>
+      <c r="O92" s="5" t="str">
+        <f t="shared" si="56"/>
+        <v>9.58%</v>
       </c>
     </row>
     <row r="93">
@@ -3121,10 +4262,10 @@
     </row>
     <row r="95">
       <c r="A95" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="96">
@@ -3180,32 +4321,32 @@
     </row>
     <row r="117">
       <c r="E117" s="8" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="118">
       <c r="F118" s="8">
         <v>1.0</v>
       </c>
-      <c r="G118" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="H118" s="14">
+      <c r="G118" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="H118" s="19">
         <v>86.0</v>
       </c>
-      <c r="I118" s="15">
+      <c r="I118" s="20">
         <v>0.0055</v>
       </c>
-      <c r="J118" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="K118" s="16">
+      <c r="J118" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K118" s="21">
         <v>556.0</v>
       </c>
-      <c r="L118" s="17">
+      <c r="L118" s="22">
         <v>0.0354</v>
       </c>
     </row>
@@ -3213,48 +4354,48 @@
       <c r="F119" s="8">
         <v>2.0</v>
       </c>
-      <c r="G119" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="H119" s="14">
+      <c r="G119" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H119" s="19">
         <v>1407.0</v>
       </c>
-      <c r="I119" s="15">
+      <c r="I119" s="20">
         <v>0.0895</v>
       </c>
-      <c r="J119" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="K119" s="16">
+      <c r="J119" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="K119" s="21">
         <v>937.0</v>
       </c>
-      <c r="L119" s="17">
+      <c r="L119" s="22">
         <v>0.0596</v>
       </c>
     </row>
     <row r="120">
-      <c r="E120" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F120" s="18">
+      <c r="E120" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F120" s="23">
         <v>3.0</v>
       </c>
-      <c r="G120" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H120" s="14">
+      <c r="G120" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H120" s="19">
         <v>1487.0</v>
       </c>
-      <c r="I120" s="15">
+      <c r="I120" s="20">
         <v>0.095</v>
       </c>
-      <c r="J120" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="K120" s="16">
+      <c r="J120" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="K120" s="21">
         <v>1487.0</v>
       </c>
-      <c r="L120" s="17">
+      <c r="L120" s="22">
         <v>0.095</v>
       </c>
     </row>
@@ -3262,267 +4403,267 @@
       <c r="F121" s="8">
         <v>4.0</v>
       </c>
-      <c r="G121" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H121" s="14">
+      <c r="G121" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H121" s="19">
         <v>10294.0</v>
       </c>
-      <c r="I121" s="15">
+      <c r="I121" s="20">
         <v>0.6548</v>
       </c>
-      <c r="J121" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="K121" s="16">
+      <c r="J121" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="K121" s="21">
         <v>3309.0</v>
       </c>
-      <c r="L121" s="17">
+      <c r="L121" s="22">
         <v>0.2105</v>
       </c>
     </row>
     <row r="122">
       <c r="E122" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F122" s="8">
         <v>5.0</v>
       </c>
-      <c r="G122" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H122" s="14">
+      <c r="G122" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H122" s="19">
         <v>2446.0</v>
       </c>
-      <c r="I122" s="15">
+      <c r="I122" s="20">
         <v>0.1556</v>
       </c>
-      <c r="J122" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="K122" s="16">
+      <c r="J122" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K122" s="21">
         <v>9431.0</v>
       </c>
-      <c r="L122" s="17">
+      <c r="L122" s="22">
         <v>0.6</v>
       </c>
     </row>
     <row r="123">
-      <c r="G123" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H123" s="19">
+      <c r="G123" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="H123" s="24">
         <v>795.0</v>
       </c>
-      <c r="I123" s="20">
+      <c r="I123" s="25">
         <v>0.0506</v>
       </c>
-      <c r="J123" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="K123" s="21">
+      <c r="J123" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="K123" s="26">
         <v>398.0</v>
       </c>
-      <c r="L123" s="22">
+      <c r="L123" s="27">
         <v>0.0253</v>
       </c>
     </row>
     <row r="124">
-      <c r="G124" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="H124" s="19">
+      <c r="G124" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="H124" s="24">
         <v>698.0</v>
       </c>
-      <c r="I124" s="20">
+      <c r="I124" s="25">
         <v>0.0444</v>
       </c>
-      <c r="J124" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="K124" s="21">
+      <c r="J124" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="K124" s="26">
         <v>1095.0</v>
       </c>
-      <c r="L124" s="22">
+      <c r="L124" s="27">
         <v>0.0697</v>
       </c>
     </row>
     <row r="125">
-      <c r="G125" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="H125" s="19">
+      <c r="G125" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H125" s="24">
         <v>1487.0</v>
       </c>
-      <c r="I125" s="20">
+      <c r="I125" s="25">
         <v>0.095</v>
       </c>
-      <c r="J125" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="K125" s="21">
+      <c r="J125" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="K125" s="26">
         <v>1487.0</v>
       </c>
-      <c r="L125" s="22">
+      <c r="L125" s="27">
         <v>0.095</v>
       </c>
     </row>
     <row r="126">
-      <c r="G126" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="H126" s="19">
+      <c r="G126" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H126" s="24">
         <v>2076.0</v>
       </c>
-      <c r="I126" s="20">
+      <c r="I126" s="25">
         <v>0.1321</v>
       </c>
-      <c r="J126" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="K126" s="21">
+      <c r="J126" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="K126" s="26">
         <v>4607.0</v>
       </c>
-      <c r="L126" s="22">
+      <c r="L126" s="27">
         <v>0.2931</v>
       </c>
     </row>
     <row r="127">
-      <c r="G127" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H127" s="19">
+      <c r="G127" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="H127" s="24">
         <v>10664.0</v>
       </c>
-      <c r="I127" s="20">
+      <c r="I127" s="25">
         <v>0.6771</v>
       </c>
-      <c r="J127" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="K127" s="21">
+      <c r="J127" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="K127" s="26">
         <v>8133.0</v>
       </c>
-      <c r="L127" s="22">
+      <c r="L127" s="27">
         <v>0.5174</v>
       </c>
     </row>
     <row r="128">
-      <c r="G128" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="H128" s="23">
+      <c r="G128" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="H128" s="28">
         <v>63.0</v>
       </c>
-      <c r="I128" s="24">
+      <c r="I128" s="29">
         <v>0.004</v>
       </c>
       <c r="J128" s="8"/>
     </row>
     <row r="129">
-      <c r="G129" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="H129" s="23">
+      <c r="G129" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="H129" s="28">
         <v>493.0</v>
       </c>
-      <c r="I129" s="24">
+      <c r="I129" s="29">
         <v>0.0314</v>
       </c>
     </row>
     <row r="130">
       <c r="F130" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G130" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="H130" s="23">
+        <v>83</v>
+      </c>
+      <c r="G130" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H130" s="28">
         <v>5733.0</v>
       </c>
-      <c r="I130" s="24">
+      <c r="I130" s="29">
         <v>0.3619</v>
       </c>
     </row>
     <row r="131">
       <c r="F131" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G131" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="H131" s="23">
+      <c r="G131" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="H131" s="28">
         <v>7779.0</v>
       </c>
-      <c r="I131" s="24">
+      <c r="I131" s="29">
         <v>0.4786</v>
       </c>
     </row>
     <row r="132">
       <c r="F132" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G132" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="H132" s="23">
+      <c r="G132" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="H132" s="28">
         <v>1652.0</v>
       </c>
-      <c r="I132" s="24">
+      <c r="I132" s="29">
         <v>0.1003</v>
       </c>
     </row>
     <row r="136">
       <c r="F136" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G136" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H136" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I136" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="137">
       <c r="F137" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G137" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H137" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="138">
       <c r="F138" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G138" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H138" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I138" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="I138" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="139">
       <c r="F139" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G139" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H139" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I139" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the analysis excel sheet with some improvements
</commit_message>
<xml_diff>
--- a/group10.Code/analysis/Data Analysis Amazon.xlsx
+++ b/group10.Code/analysis/Data Analysis Amazon.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
   <si>
     <t>Total</t>
   </si>
@@ -61,142 +61,139 @@
     <t>Rating vs Sentiment Matrix</t>
   </si>
   <si>
-    <t>🠗 Sentiment</t>
+    <t>🠗 Score</t>
+  </si>
+  <si>
+    <t>🠖 Sentiment</t>
+  </si>
+  <si>
+    <t>13  121  497  79  15</t>
+  </si>
+  <si>
+    <t>6  95  465  110  8</t>
+  </si>
+  <si>
+    <t>15  69  749  427  65</t>
+  </si>
+  <si>
+    <t>10  71  1154  1486  254</t>
+  </si>
+  <si>
+    <t>19  138  2824  5422  1235</t>
+  </si>
+  <si>
+    <t>2  16  49  6  4</t>
+  </si>
+  <si>
+    <t>2  14  43  9  1</t>
+  </si>
+  <si>
+    <t>2  7  75  54  13</t>
+  </si>
+  <si>
+    <t>2  5  145  170  44</t>
+  </si>
+  <si>
+    <t>6  16  330  658  184</t>
+  </si>
+  <si>
+    <t>2  10  31  7  0</t>
+  </si>
+  <si>
+    <t>0  4  42  7  1</t>
+  </si>
+  <si>
+    <t>2  5  69  33  3</t>
+  </si>
+  <si>
+    <t>0  6  130  206  22</t>
+  </si>
+  <si>
+    <t>3  13  387  733  124</t>
+  </si>
+  <si>
+    <t>0  8  20  6  2</t>
+  </si>
+  <si>
+    <t>1  7  25  11  0</t>
+  </si>
+  <si>
+    <t>2  2  72  40  4</t>
+  </si>
+  <si>
+    <t>0  3  161  239  23</t>
+  </si>
+  <si>
+    <t>2  10  371  738  124</t>
+  </si>
+  <si>
+    <t>7  46  149  30  3</t>
+  </si>
+  <si>
+    <t>1  29  138  32  3</t>
+  </si>
+  <si>
+    <t>7  36  227  120  21</t>
+  </si>
+  <si>
+    <t>7  38  325  329  79</t>
+  </si>
+  <si>
+    <t>8  74  751  1225  342</t>
+  </si>
+  <si>
+    <t>0  15  128  12  4</t>
+  </si>
+  <si>
+    <t>0  10  71  13  0</t>
+  </si>
+  <si>
+    <t>0  6  110  48  3</t>
+  </si>
+  <si>
+    <t>0  9  166  182  23</t>
+  </si>
+  <si>
+    <t>0  12  432  711  132</t>
+  </si>
+  <si>
+    <t>0  8  43  8  1</t>
+  </si>
+  <si>
+    <t>2  12  63  22  1</t>
+  </si>
+  <si>
+    <t>0  7  82  70  6</t>
+  </si>
+  <si>
+    <t>1  7  118  192  38</t>
+  </si>
+  <si>
+    <t>0  2  245  751  229</t>
+  </si>
+  <si>
+    <t>2  18  77  10  1</t>
+  </si>
+  <si>
+    <t>0  19  83  16  2</t>
+  </si>
+  <si>
+    <t>2  6  114  62  15</t>
+  </si>
+  <si>
+    <t>0  3  109  168  25</t>
+  </si>
+  <si>
+    <t>0  11  308  606  100</t>
+  </si>
+  <si>
+    <t>Graphs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Walmart Data Analysis Graphs will be located in another excel sheet.</t>
   </si>
   <si>
     <t>Sentiment</t>
-  </si>
-  <si>
-    <t>🠖 Score</t>
-  </si>
-  <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>13  121  497  79  15</t>
-  </si>
-  <si>
-    <t>6  95  465  110  8</t>
-  </si>
-  <si>
-    <t>15  69  749  427  65</t>
-  </si>
-  <si>
-    <t>10  71  1154  1486  254</t>
-  </si>
-  <si>
-    <t>19  138  2824  5422  1235</t>
-  </si>
-  <si>
-    <t>2  16  49  6  4</t>
-  </si>
-  <si>
-    <t>2  14  43  9  1</t>
-  </si>
-  <si>
-    <t>2  7  75  54  13</t>
-  </si>
-  <si>
-    <t>2  5  145  170  44</t>
-  </si>
-  <si>
-    <t>6  16  330  658  184</t>
-  </si>
-  <si>
-    <t>2  10  31  7  0</t>
-  </si>
-  <si>
-    <t>0  4  42  7  1</t>
-  </si>
-  <si>
-    <t>2  5  69  33  3</t>
-  </si>
-  <si>
-    <t>0  6  130  206  22</t>
-  </si>
-  <si>
-    <t>3  13  387  733  124</t>
-  </si>
-  <si>
-    <t>0  8  20  6  2</t>
-  </si>
-  <si>
-    <t>1  7  25  11  0</t>
-  </si>
-  <si>
-    <t>2  2  72  40  4</t>
-  </si>
-  <si>
-    <t>0  3  161  239  23</t>
-  </si>
-  <si>
-    <t>2  10  371  738  124</t>
-  </si>
-  <si>
-    <t>7  46  149  30  3</t>
-  </si>
-  <si>
-    <t>1  29  138  32  3</t>
-  </si>
-  <si>
-    <t>7  36  227  120  21</t>
-  </si>
-  <si>
-    <t>7  38  325  329  79</t>
-  </si>
-  <si>
-    <t>8  74  751  1225  342</t>
-  </si>
-  <si>
-    <t>0  15  128  12  4</t>
-  </si>
-  <si>
-    <t>0  10  71  13  0</t>
-  </si>
-  <si>
-    <t>0  6  110  48  3</t>
-  </si>
-  <si>
-    <t>0  9  166  182  23</t>
-  </si>
-  <si>
-    <t>0  12  432  711  132</t>
-  </si>
-  <si>
-    <t>0  8  43  8  1</t>
-  </si>
-  <si>
-    <t>2  12  63  22  1</t>
-  </si>
-  <si>
-    <t>0  7  82  70  6</t>
-  </si>
-  <si>
-    <t>1  7  118  192  38</t>
-  </si>
-  <si>
-    <t>0  2  245  751  229</t>
-  </si>
-  <si>
-    <t>2  18  77  10  1</t>
-  </si>
-  <si>
-    <t>0  19  83  16  2</t>
-  </si>
-  <si>
-    <t>2  6  114  62  15</t>
-  </si>
-  <si>
-    <t>0  3  109  168  25</t>
-  </si>
-  <si>
-    <t>0  11  308  606  100</t>
-  </si>
-  <si>
-    <t>Graphs</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Walmart Data Analysis Graphs will be located in another excel sheet.</t>
   </si>
   <si>
     <t>Estimated Score</t>
@@ -338,10 +335,11 @@
     </font>
     <font>
       <b/>
-      <color rgb="FFAEAEAE"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <color rgb="FFAEAEAE"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -401,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -433,7 +431,7 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -443,16 +441,10 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1744,9 +1736,7 @@
       <c r="C30" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="K30" s="11"/>
       <c r="L30" s="12"/>
       <c r="M30" s="12"/>
       <c r="N30" s="12"/>
@@ -1754,7 +1744,7 @@
     </row>
     <row r="31">
       <c r="B31" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" s="2">
         <v>1.0</v>
@@ -1771,9 +1761,7 @@
       <c r="G31" s="2">
         <v>5.0</v>
       </c>
-      <c r="J31" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="J31" s="11"/>
       <c r="K31" s="13">
         <v>1.0</v>
       </c>
@@ -1815,13 +1803,13 @@
         <v>15</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" s="16">
+        <v>18</v>
+      </c>
+      <c r="J32" s="13">
         <v>1.0</v>
       </c>
       <c r="K32" s="5" t="str">
-        <f t="shared" ref="K32:O32" si="17">ROUNDUP((C32/$K5), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K32:O32" si="17">ROUNDUP((C32/$K5),4)*100&amp;"%"</f>
         <v>1.75%</v>
       </c>
       <c r="L32" s="5" t="str">
@@ -1842,7 +1830,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="17"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="2">
         <v>2.0</v>
       </c>
@@ -1867,13 +1855,13 @@
         <v>8</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J33" s="13">
         <v>2.0</v>
       </c>
       <c r="K33" s="5" t="str">
-        <f t="shared" ref="K33:O33" si="18">ROUNDUP((C33/$K6), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K33:O33" si="18">ROUNDUP((C33/$K6),4)*100&amp;"%"</f>
         <v>0.87%</v>
       </c>
       <c r="L33" s="5" t="str">
@@ -1919,13 +1907,13 @@
         <v>65</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J34" s="13">
         <v>3.0</v>
       </c>
       <c r="K34" s="5" t="str">
-        <f t="shared" ref="K34:O34" si="19">ROUNDUP((C34/$K7), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K34:O34" si="19">ROUNDUP((C34/$K7),4)*100&amp;"%"</f>
         <v>1.1%</v>
       </c>
       <c r="L34" s="5" t="str">
@@ -1971,13 +1959,13 @@
         <v>254</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J35" s="13">
         <v>4.0</v>
       </c>
       <c r="K35" s="5" t="str">
-        <f t="shared" ref="K35:O35" si="20">ROUNDUP((C35/$K8), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K35:O35" si="20">ROUNDUP((C35/$K8),4)*100&amp;"%"</f>
         <v>0.34%</v>
       </c>
       <c r="L35" s="5" t="str">
@@ -2023,13 +2011,13 @@
         <v>1235</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J36" s="13">
         <v>5.0</v>
       </c>
       <c r="K36" s="5" t="str">
-        <f t="shared" ref="K36:O36" si="21">ROUNDUP((C36/$K9), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K36:O36" si="21">ROUNDUP((C36/$K9),4)*100&amp;"%"</f>
         <v>0.2%</v>
       </c>
       <c r="L36" s="5" t="str">
@@ -2059,9 +2047,7 @@
       <c r="C38" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K38" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="K38" s="11"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
@@ -2069,7 +2055,7 @@
     </row>
     <row r="39">
       <c r="B39" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="2">
         <v>1.0</v>
@@ -2086,9 +2072,7 @@
       <c r="G39" s="2">
         <v>5.0</v>
       </c>
-      <c r="J39" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="J39" s="11"/>
       <c r="K39" s="13">
         <v>1.0</v>
       </c>
@@ -2130,13 +2114,13 @@
         <v>4</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J40" s="13">
         <v>1.0</v>
       </c>
       <c r="K40" s="5" t="str">
-        <f t="shared" ref="K40:O40" si="22">ROUNDUP((C40/$L5), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K40:O40" si="22">ROUNDUP((C40/$L5),4)*100&amp;"%"</f>
         <v>2.6%</v>
       </c>
       <c r="L40" s="5" t="str">
@@ -2157,7 +2141,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="17"/>
+      <c r="A41" s="16"/>
       <c r="B41" s="2">
         <v>2.0</v>
       </c>
@@ -2182,13 +2166,13 @@
         <v>1</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J41" s="13">
         <v>2.0</v>
       </c>
       <c r="K41" s="5" t="str">
-        <f t="shared" ref="K41:O41" si="23">ROUNDUP((C41/$L6), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K41:O41" si="23">ROUNDUP((C41/$L6),4)*100&amp;"%"</f>
         <v>2.86%</v>
       </c>
       <c r="L41" s="5" t="str">
@@ -2234,13 +2218,13 @@
         <v>13</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J42" s="13">
         <v>3.0</v>
       </c>
       <c r="K42" s="5" t="str">
-        <f t="shared" ref="K42:O42" si="24">ROUNDUP((C42/$L7), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K42:O42" si="24">ROUNDUP((C42/$L7),4)*100&amp;"%"</f>
         <v>1.27%</v>
       </c>
       <c r="L42" s="5" t="str">
@@ -2286,13 +2270,13 @@
         <v>44</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J43" s="13">
         <v>4.0</v>
       </c>
       <c r="K43" s="5" t="str">
-        <f t="shared" ref="K43:O43" si="25">ROUNDUP((C43/$L8), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K43:O43" si="25">ROUNDUP((C43/$L8),4)*100&amp;"%"</f>
         <v>0.54%</v>
       </c>
       <c r="L43" s="5" t="str">
@@ -2338,13 +2322,13 @@
         <v>184</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J44" s="13">
         <v>5.0</v>
       </c>
       <c r="K44" s="5" t="str">
-        <f t="shared" ref="K44:O44" si="26">ROUNDUP((C44/$L9), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K44:O44" si="26">ROUNDUP((C44/$L9),4)*100&amp;"%"</f>
         <v>0.5%</v>
       </c>
       <c r="L44" s="5" t="str">
@@ -2374,9 +2358,7 @@
       <c r="C46" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K46" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="K46" s="11"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12"/>
       <c r="N46" s="12"/>
@@ -2384,7 +2366,7 @@
     </row>
     <row r="47">
       <c r="B47" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C47" s="2">
         <v>1.0</v>
@@ -2401,9 +2383,7 @@
       <c r="G47" s="2">
         <v>5.0</v>
       </c>
-      <c r="J47" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="J47" s="11"/>
       <c r="K47" s="13">
         <v>1.0</v>
       </c>
@@ -2445,13 +2425,13 @@
         <v>0</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J48" s="13">
         <v>1.0</v>
       </c>
       <c r="K48" s="5" t="str">
-        <f t="shared" ref="K48:O48" si="27">ROUNDUP((C48/$M5), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K48:O48" si="27">ROUNDUP((C48/$M5),4)*100&amp;"%"</f>
         <v>3.93%</v>
       </c>
       <c r="L48" s="5" t="str">
@@ -2472,7 +2452,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="17"/>
+      <c r="A49" s="16"/>
       <c r="B49" s="2">
         <v>2.0</v>
       </c>
@@ -2497,13 +2477,13 @@
         <v>1</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J49" s="13">
         <v>2.0</v>
       </c>
       <c r="K49" s="5" t="str">
-        <f t="shared" ref="K49:O49" si="28">ROUNDUP((C49/$M6), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K49:O49" si="28">ROUNDUP((C49/$M6),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L49" s="5" t="str">
@@ -2549,13 +2529,13 @@
         <v>3</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J50" s="13">
         <v>3.0</v>
       </c>
       <c r="K50" s="5" t="str">
-        <f t="shared" ref="K50:O50" si="29">ROUNDUP((C50/$M7), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K50:O50" si="29">ROUNDUP((C50/$M7),4)*100&amp;"%"</f>
         <v>1.76%</v>
       </c>
       <c r="L50" s="5" t="str">
@@ -2601,13 +2581,13 @@
         <v>22</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J51" s="13">
         <v>4.0</v>
       </c>
       <c r="K51" s="5" t="str">
-        <f t="shared" ref="K51:O51" si="30">ROUNDUP((C51/$M8), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K51:O51" si="30">ROUNDUP((C51/$M8),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L51" s="5" t="str">
@@ -2653,13 +2633,13 @@
         <v>124</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J52" s="13">
         <v>5.0</v>
       </c>
       <c r="K52" s="5" t="str">
-        <f t="shared" ref="K52:O52" si="31">ROUNDUP((C52/$M9), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K52:O52" si="31">ROUNDUP((C52/$M9),4)*100&amp;"%"</f>
         <v>0.24%</v>
       </c>
       <c r="L52" s="5" t="str">
@@ -2689,9 +2669,7 @@
       <c r="C54" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K54" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="K54" s="11"/>
       <c r="L54" s="12"/>
       <c r="M54" s="12"/>
       <c r="N54" s="12"/>
@@ -2699,7 +2677,7 @@
     </row>
     <row r="55">
       <c r="B55" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C55" s="2">
         <v>1.0</v>
@@ -2716,22 +2694,20 @@
       <c r="G55" s="2">
         <v>5.0</v>
       </c>
-      <c r="J55" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K55" s="16">
+      <c r="J55" s="11"/>
+      <c r="K55" s="13">
         <v>1.0</v>
       </c>
-      <c r="L55" s="16">
+      <c r="L55" s="13">
         <v>2.0</v>
       </c>
-      <c r="M55" s="16">
+      <c r="M55" s="13">
         <v>3.0</v>
       </c>
-      <c r="N55" s="16">
+      <c r="N55" s="13">
         <v>4.0</v>
       </c>
-      <c r="O55" s="16">
+      <c r="O55" s="13">
         <v>5.0</v>
       </c>
     </row>
@@ -2760,13 +2736,13 @@
         <v>2</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J56" s="16">
+        <v>33</v>
+      </c>
+      <c r="J56" s="13">
         <v>1.0</v>
       </c>
       <c r="K56" s="5" t="str">
-        <f t="shared" ref="K56:O56" si="32">ROUNDUP((C56/$N5), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K56:O56" si="32">ROUNDUP((C56/$N5),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L56" s="5" t="str">
@@ -2787,7 +2763,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="17"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="2">
         <v>2.0</v>
       </c>
@@ -2812,13 +2788,13 @@
         <v>0</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="J57" s="16">
+        <v>34</v>
+      </c>
+      <c r="J57" s="13">
         <v>2.0</v>
       </c>
       <c r="K57" s="5" t="str">
-        <f t="shared" ref="K57:O57" si="33">ROUNDUP((C57/$N6), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K57:O57" si="33">ROUNDUP((C57/$N6),4)*100&amp;"%"</f>
         <v>2.18%</v>
       </c>
       <c r="L57" s="5" t="str">
@@ -2864,13 +2840,13 @@
         <v>4</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="J58" s="16">
+        <v>35</v>
+      </c>
+      <c r="J58" s="13">
         <v>3.0</v>
       </c>
       <c r="K58" s="5" t="str">
-        <f t="shared" ref="K58:O58" si="34">ROUNDUP((C58/$N7), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K58:O58" si="34">ROUNDUP((C58/$N7),4)*100&amp;"%"</f>
         <v>1.59%</v>
       </c>
       <c r="L58" s="5" t="str">
@@ -2916,13 +2892,13 @@
         <v>23</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="J59" s="16">
+        <v>36</v>
+      </c>
+      <c r="J59" s="13">
         <v>4.0</v>
       </c>
       <c r="K59" s="5" t="str">
-        <f t="shared" ref="K59:O59" si="35">ROUNDUP((C59/$N8), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K59:O59" si="35">ROUNDUP((C59/$N8),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L59" s="5" t="str">
@@ -2968,13 +2944,13 @@
         <v>124</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="J60" s="16">
+        <v>37</v>
+      </c>
+      <c r="J60" s="13">
         <v>5.0</v>
       </c>
       <c r="K60" s="5" t="str">
-        <f t="shared" ref="K60:O60" si="36">ROUNDUP((C60/$N9), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K60:O60" si="36">ROUNDUP((C60/$N9),4)*100&amp;"%"</f>
         <v>0.16%</v>
       </c>
       <c r="L60" s="5" t="str">
@@ -3004,9 +2980,7 @@
       <c r="C62" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K62" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="K62" s="11"/>
       <c r="L62" s="12"/>
       <c r="M62" s="12"/>
       <c r="N62" s="12"/>
@@ -3014,7 +2988,7 @@
     </row>
     <row r="63">
       <c r="B63" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C63" s="2">
         <v>1.0</v>
@@ -3031,22 +3005,20 @@
       <c r="G63" s="2">
         <v>5.0</v>
       </c>
-      <c r="J63" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K63" s="16">
+      <c r="J63" s="11"/>
+      <c r="K63" s="13">
         <v>1.0</v>
       </c>
-      <c r="L63" s="16">
+      <c r="L63" s="13">
         <v>2.0</v>
       </c>
-      <c r="M63" s="16">
+      <c r="M63" s="13">
         <v>3.0</v>
       </c>
-      <c r="N63" s="16">
+      <c r="N63" s="13">
         <v>4.0</v>
       </c>
-      <c r="O63" s="16">
+      <c r="O63" s="13">
         <v>5.0</v>
       </c>
     </row>
@@ -3075,13 +3047,13 @@
         <v>3</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="J64" s="16">
+        <v>38</v>
+      </c>
+      <c r="J64" s="13">
         <v>1.0</v>
       </c>
       <c r="K64" s="5" t="str">
-        <f t="shared" ref="K64:O64" si="37">ROUNDUP((C64/$O5), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K64:O64" si="37">ROUNDUP((C64/$O5),4)*100&amp;"%"</f>
         <v>2.91%</v>
       </c>
       <c r="L64" s="5" t="str">
@@ -3102,7 +3074,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="17"/>
+      <c r="A65" s="16"/>
       <c r="B65" s="2">
         <v>2.0</v>
       </c>
@@ -3127,13 +3099,13 @@
         <v>3</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J65" s="16">
+        <v>39</v>
+      </c>
+      <c r="J65" s="13">
         <v>2.0</v>
       </c>
       <c r="K65" s="5" t="str">
-        <f t="shared" ref="K65:O65" si="38">ROUNDUP((C65/$O6), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K65:O65" si="38">ROUNDUP((C65/$O6),4)*100&amp;"%"</f>
         <v>0.49%</v>
       </c>
       <c r="L65" s="5" t="str">
@@ -3179,13 +3151,13 @@
         <v>21</v>
       </c>
       <c r="H66" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="J66" s="16">
+        <v>40</v>
+      </c>
+      <c r="J66" s="13">
         <v>3.0</v>
       </c>
       <c r="K66" s="5" t="str">
-        <f t="shared" ref="K66:O66" si="39">ROUNDUP((C66/$O7), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K66:O66" si="39">ROUNDUP((C66/$O7),4)*100&amp;"%"</f>
         <v>1.66%</v>
       </c>
       <c r="L66" s="5" t="str">
@@ -3231,13 +3203,13 @@
         <v>79</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="J67" s="16">
+        <v>41</v>
+      </c>
+      <c r="J67" s="13">
         <v>4.0</v>
       </c>
       <c r="K67" s="5" t="str">
-        <f t="shared" ref="K67:O67" si="40">ROUNDUP((C67/$O8), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K67:O67" si="40">ROUNDUP((C67/$O8),4)*100&amp;"%"</f>
         <v>0.89%</v>
       </c>
       <c r="L67" s="5" t="str">
@@ -3283,13 +3255,13 @@
         <v>342</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J68" s="16">
+        <v>42</v>
+      </c>
+      <c r="J68" s="13">
         <v>5.0</v>
       </c>
       <c r="K68" s="5" t="str">
-        <f t="shared" ref="K68:O68" si="41">ROUNDUP((C68/$O9), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K68:O68" si="41">ROUNDUP((C68/$O9),4)*100&amp;"%"</f>
         <v>0.33%</v>
       </c>
       <c r="L68" s="5" t="str">
@@ -3319,9 +3291,7 @@
       <c r="C70" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K70" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="K70" s="11"/>
       <c r="L70" s="12"/>
       <c r="M70" s="12"/>
       <c r="N70" s="12"/>
@@ -3329,7 +3299,7 @@
     </row>
     <row r="71">
       <c r="B71" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C71" s="2">
         <v>1.0</v>
@@ -3346,22 +3316,20 @@
       <c r="G71" s="2">
         <v>5.0</v>
       </c>
-      <c r="J71" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K71" s="16">
+      <c r="J71" s="11"/>
+      <c r="K71" s="13">
         <v>1.0</v>
       </c>
-      <c r="L71" s="16">
+      <c r="L71" s="13">
         <v>2.0</v>
       </c>
-      <c r="M71" s="16">
+      <c r="M71" s="13">
         <v>3.0</v>
       </c>
-      <c r="N71" s="16">
+      <c r="N71" s="13">
         <v>4.0</v>
       </c>
-      <c r="O71" s="16">
+      <c r="O71" s="13">
         <v>5.0</v>
       </c>
     </row>
@@ -3390,13 +3358,13 @@
         <v>4</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="J72" s="16">
+        <v>43</v>
+      </c>
+      <c r="J72" s="13">
         <v>1.0</v>
       </c>
       <c r="K72" s="5" t="str">
-        <f t="shared" ref="K72:O72" si="42">ROUNDUP((C72/$P5), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K72:O72" si="42">ROUNDUP((C72/$P5),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L72" s="5" t="str">
@@ -3417,7 +3385,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="17"/>
+      <c r="A73" s="16"/>
       <c r="B73" s="2">
         <v>2.0</v>
       </c>
@@ -3442,13 +3410,13 @@
         <v>0</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="J73" s="16">
+        <v>44</v>
+      </c>
+      <c r="J73" s="13">
         <v>2.0</v>
       </c>
       <c r="K73" s="5" t="str">
-        <f t="shared" ref="K73:O73" si="43">ROUNDUP((C73/$P6), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K73:O73" si="43">ROUNDUP((C73/$P6),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L73" s="5" t="str">
@@ -3494,13 +3462,13 @@
         <v>3</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="J74" s="16">
+        <v>45</v>
+      </c>
+      <c r="J74" s="13">
         <v>3.0</v>
       </c>
       <c r="K74" s="5" t="str">
-        <f t="shared" ref="K74:O74" si="44">ROUNDUP((C74/$P7), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K74:O74" si="44">ROUNDUP((C74/$P7),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L74" s="5" t="str">
@@ -3546,13 +3514,13 @@
         <v>23</v>
       </c>
       <c r="H75" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="J75" s="16">
+        <v>46</v>
+      </c>
+      <c r="J75" s="13">
         <v>4.0</v>
       </c>
       <c r="K75" s="5" t="str">
-        <f t="shared" ref="K75:O75" si="45">ROUNDUP((C75/$P8), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K75:O75" si="45">ROUNDUP((C75/$P8),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L75" s="5" t="str">
@@ -3598,13 +3566,13 @@
         <v>132</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J76" s="16">
+        <v>47</v>
+      </c>
+      <c r="J76" s="13">
         <v>5.0</v>
       </c>
       <c r="K76" s="5" t="str">
-        <f t="shared" ref="K76:O76" si="46">ROUNDUP((C76/$P9), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K76:O76" si="46">ROUNDUP((C76/$P9),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L76" s="5" t="str">
@@ -3634,9 +3602,7 @@
       <c r="C78" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K78" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="K78" s="11"/>
       <c r="L78" s="12"/>
       <c r="M78" s="12"/>
       <c r="N78" s="12"/>
@@ -3644,7 +3610,7 @@
     </row>
     <row r="79">
       <c r="B79" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C79" s="2">
         <v>1.0</v>
@@ -3661,9 +3627,7 @@
       <c r="G79" s="2">
         <v>5.0</v>
       </c>
-      <c r="J79" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="J79" s="11"/>
       <c r="K79" s="13">
         <v>1.0</v>
       </c>
@@ -3705,13 +3669,13 @@
         <v>1</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J80" s="13">
         <v>1.0</v>
       </c>
       <c r="K80" s="5" t="str">
-        <f t="shared" ref="K80:O80" si="47">ROUNDUP((C80/$Q5), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K80:O80" si="47">ROUNDUP((C80/$Q5),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L80" s="5" t="str">
@@ -3732,7 +3696,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="17"/>
+      <c r="A81" s="16"/>
       <c r="B81" s="2">
         <v>2.0</v>
       </c>
@@ -3757,13 +3721,13 @@
         <v>1</v>
       </c>
       <c r="H81" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J81" s="13">
         <v>2.0</v>
       </c>
       <c r="K81" s="5" t="str">
-        <f t="shared" ref="K81:O81" si="48">ROUNDUP((C81/$Q6), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K81:O81" si="48">ROUNDUP((C81/$Q6),4)*100&amp;"%"</f>
         <v>2%</v>
       </c>
       <c r="L81" s="5" t="str">
@@ -3809,13 +3773,13 @@
         <v>6</v>
       </c>
       <c r="H82" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J82" s="13">
         <v>3.0</v>
       </c>
       <c r="K82" s="5" t="str">
-        <f t="shared" ref="K82:O82" si="49">ROUNDUP((C82/$Q7), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K82:O82" si="49">ROUNDUP((C82/$Q7),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L82" s="5" t="str">
@@ -3861,13 +3825,13 @@
         <v>38</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J83" s="13">
         <v>4.0</v>
       </c>
       <c r="K83" s="5" t="str">
-        <f t="shared" ref="K83:O83" si="50">ROUNDUP((C83/$Q8), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K83:O83" si="50">ROUNDUP((C83/$Q8),4)*100&amp;"%"</f>
         <v>0.28%</v>
       </c>
       <c r="L83" s="5" t="str">
@@ -3913,13 +3877,13 @@
         <v>229</v>
       </c>
       <c r="H84" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J84" s="13">
         <v>5.0</v>
       </c>
       <c r="K84" s="5" t="str">
-        <f t="shared" ref="K84:O84" si="51">ROUNDUP((C84/$Q9), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K84:O84" si="51">ROUNDUP((C84/$Q9),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L84" s="5" t="str">
@@ -3949,9 +3913,7 @@
       <c r="C86" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K86" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="K86" s="11"/>
       <c r="L86" s="12"/>
       <c r="M86" s="12"/>
       <c r="N86" s="12"/>
@@ -3959,7 +3921,7 @@
     </row>
     <row r="87">
       <c r="B87" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C87" s="2">
         <v>1.0</v>
@@ -3976,9 +3938,7 @@
       <c r="G87" s="2">
         <v>5.0</v>
       </c>
-      <c r="J87" s="18" t="s">
-        <v>19</v>
-      </c>
+      <c r="J87" s="11"/>
       <c r="K87" s="13">
         <v>1.0</v>
       </c>
@@ -4020,13 +3980,13 @@
         <v>1</v>
       </c>
       <c r="H88" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="J88" s="16">
+        <v>53</v>
+      </c>
+      <c r="J88" s="13">
         <v>1.0</v>
       </c>
       <c r="K88" s="5" t="str">
-        <f t="shared" ref="K88:O88" si="52">ROUNDUP((C88/$R5), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K88:O88" si="52">ROUNDUP((C88/$R5),4)*100&amp;"%"</f>
         <v>1.82%</v>
       </c>
       <c r="L88" s="5" t="str">
@@ -4047,7 +4007,7 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="17"/>
+      <c r="A89" s="16"/>
       <c r="B89" s="2">
         <v>2.0</v>
       </c>
@@ -4072,13 +4032,13 @@
         <v>2</v>
       </c>
       <c r="H89" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J89" s="16">
+        <v>54</v>
+      </c>
+      <c r="J89" s="13">
         <v>2.0</v>
       </c>
       <c r="K89" s="5" t="str">
-        <f t="shared" ref="K89:O89" si="53">ROUNDUP((C89/$R6), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K89:O89" si="53">ROUNDUP((C89/$R6),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L89" s="5" t="str">
@@ -4124,13 +4084,13 @@
         <v>15</v>
       </c>
       <c r="H90" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="J90" s="16">
+        <v>55</v>
+      </c>
+      <c r="J90" s="13">
         <v>3.0</v>
       </c>
       <c r="K90" s="5" t="str">
-        <f t="shared" ref="K90:O90" si="54">ROUNDUP((C90/$R7), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K90:O90" si="54">ROUNDUP((C90/$R7),4)*100&amp;"%"</f>
         <v>0.99%</v>
       </c>
       <c r="L90" s="5" t="str">
@@ -4176,13 +4136,13 @@
         <v>25</v>
       </c>
       <c r="H91" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="J91" s="16">
+        <v>56</v>
+      </c>
+      <c r="J91" s="13">
         <v>4.0</v>
       </c>
       <c r="K91" s="5" t="str">
-        <f t="shared" ref="K91:O91" si="55">ROUNDUP((C91/$R8), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K91:O91" si="55">ROUNDUP((C91/$R8),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L91" s="5" t="str">
@@ -4228,13 +4188,13 @@
         <v>100</v>
       </c>
       <c r="H92" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J92" s="13">
         <v>5.0</v>
       </c>
       <c r="K92" s="5" t="str">
-        <f t="shared" ref="K92:O92" si="56">ROUNDUP((C92/$R9), 4)*100&amp;"%"</f>
+        <f t="shared" ref="K92:O92" si="56">ROUNDUP((C92/$R9),4)*100&amp;"%"</f>
         <v>0%</v>
       </c>
       <c r="L92" s="5" t="str">
@@ -4262,10 +4222,10 @@
     </row>
     <row r="95">
       <c r="A95" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="96">
@@ -4321,32 +4281,32 @@
     </row>
     <row r="117">
       <c r="E117" s="8" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="118">
       <c r="F118" s="8">
         <v>1.0</v>
       </c>
-      <c r="G118" s="19" t="s">
+      <c r="G118" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H118" s="17">
+        <v>86.0</v>
+      </c>
+      <c r="I118" s="18">
+        <v>0.0055</v>
+      </c>
+      <c r="J118" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="H118" s="19">
-        <v>86.0</v>
-      </c>
-      <c r="I118" s="20">
-        <v>0.0055</v>
-      </c>
-      <c r="J118" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K118" s="21">
+      <c r="K118" s="19">
         <v>556.0</v>
       </c>
-      <c r="L118" s="22">
+      <c r="L118" s="20">
         <v>0.0354</v>
       </c>
     </row>
@@ -4354,48 +4314,48 @@
       <c r="F119" s="8">
         <v>2.0</v>
       </c>
-      <c r="G119" s="19" t="s">
+      <c r="G119" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H119" s="17">
+        <v>1407.0</v>
+      </c>
+      <c r="I119" s="18">
+        <v>0.0895</v>
+      </c>
+      <c r="J119" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="H119" s="19">
-        <v>1407.0</v>
-      </c>
-      <c r="I119" s="20">
-        <v>0.0895</v>
-      </c>
-      <c r="J119" s="21" t="s">
+      <c r="K119" s="19">
+        <v>937.0</v>
+      </c>
+      <c r="L119" s="20">
+        <v>0.0596</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="E120" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="K119" s="21">
-        <v>937.0</v>
-      </c>
-      <c r="L119" s="22">
-        <v>0.0596</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="E120" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F120" s="23">
+      <c r="F120" s="21">
         <v>3.0</v>
       </c>
-      <c r="G120" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="H120" s="19">
+      <c r="G120" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H120" s="17">
         <v>1487.0</v>
       </c>
-      <c r="I120" s="20">
+      <c r="I120" s="18">
         <v>0.095</v>
       </c>
-      <c r="J120" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="K120" s="21">
+      <c r="J120" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="K120" s="19">
         <v>1487.0</v>
       </c>
-      <c r="L120" s="22">
+      <c r="L120" s="20">
         <v>0.095</v>
       </c>
     </row>
@@ -4403,267 +4363,267 @@
       <c r="F121" s="8">
         <v>4.0</v>
       </c>
-      <c r="G121" s="19" t="s">
+      <c r="G121" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H121" s="17">
+        <v>10294.0</v>
+      </c>
+      <c r="I121" s="18">
+        <v>0.6548</v>
+      </c>
+      <c r="J121" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="H121" s="19">
-        <v>10294.0</v>
-      </c>
-      <c r="I121" s="20">
-        <v>0.6548</v>
-      </c>
-      <c r="J121" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K121" s="21">
+      <c r="K121" s="19">
         <v>3309.0</v>
       </c>
-      <c r="L121" s="22">
+      <c r="L121" s="20">
         <v>0.2105</v>
       </c>
     </row>
     <row r="122">
       <c r="E122" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F122" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="G122" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F122" s="8">
-        <v>5.0</v>
-      </c>
-      <c r="G122" s="19" t="s">
+      <c r="H122" s="17">
+        <v>2446.0</v>
+      </c>
+      <c r="I122" s="18">
+        <v>0.1556</v>
+      </c>
+      <c r="J122" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H122" s="19">
-        <v>2446.0</v>
-      </c>
-      <c r="I122" s="20">
-        <v>0.1556</v>
-      </c>
-      <c r="J122" s="21" t="s">
+      <c r="K122" s="19">
+        <v>9431.0</v>
+      </c>
+      <c r="L122" s="20">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="G123" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="K122" s="21">
-        <v>9431.0</v>
-      </c>
-      <c r="L122" s="22">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="G123" s="24" t="s">
+      <c r="H123" s="22">
+        <v>795.0</v>
+      </c>
+      <c r="I123" s="23">
+        <v>0.0506</v>
+      </c>
+      <c r="J123" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="H123" s="24">
-        <v>795.0</v>
-      </c>
-      <c r="I123" s="25">
-        <v>0.0506</v>
-      </c>
-      <c r="J123" s="26" t="s">
+      <c r="K123" s="24">
+        <v>398.0</v>
+      </c>
+      <c r="L123" s="25">
+        <v>0.0253</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="G124" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="K123" s="26">
-        <v>398.0</v>
-      </c>
-      <c r="L123" s="27">
-        <v>0.0253</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="G124" s="24" t="s">
+      <c r="H124" s="22">
+        <v>698.0</v>
+      </c>
+      <c r="I124" s="23">
+        <v>0.0444</v>
+      </c>
+      <c r="J124" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="H124" s="24">
-        <v>698.0</v>
-      </c>
-      <c r="I124" s="25">
-        <v>0.0444</v>
-      </c>
-      <c r="J124" s="26" t="s">
+      <c r="K124" s="24">
+        <v>1095.0</v>
+      </c>
+      <c r="L124" s="25">
+        <v>0.0697</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="G125" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H125" s="22">
+        <v>1487.0</v>
+      </c>
+      <c r="I125" s="23">
+        <v>0.095</v>
+      </c>
+      <c r="J125" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="K125" s="24">
+        <v>1487.0</v>
+      </c>
+      <c r="L125" s="25">
+        <v>0.095</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="G126" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="K124" s="26">
-        <v>1095.0</v>
-      </c>
-      <c r="L124" s="27">
-        <v>0.0697</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="G125" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="H125" s="24">
-        <v>1487.0</v>
-      </c>
-      <c r="I125" s="25">
-        <v>0.095</v>
-      </c>
-      <c r="J125" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="K125" s="26">
-        <v>1487.0</v>
-      </c>
-      <c r="L125" s="27">
-        <v>0.095</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="G126" s="24" t="s">
+      <c r="H126" s="22">
+        <v>2076.0</v>
+      </c>
+      <c r="I126" s="23">
+        <v>0.1321</v>
+      </c>
+      <c r="J126" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H126" s="24">
-        <v>2076.0</v>
-      </c>
-      <c r="I126" s="25">
-        <v>0.1321</v>
-      </c>
-      <c r="J126" s="26" t="s">
+      <c r="K126" s="24">
+        <v>4607.0</v>
+      </c>
+      <c r="L126" s="25">
+        <v>0.2931</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="G127" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="K126" s="26">
-        <v>4607.0</v>
-      </c>
-      <c r="L126" s="27">
-        <v>0.2931</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="G127" s="24" t="s">
+      <c r="H127" s="22">
+        <v>10664.0</v>
+      </c>
+      <c r="I127" s="23">
+        <v>0.6771</v>
+      </c>
+      <c r="J127" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="H127" s="24">
-        <v>10664.0</v>
-      </c>
-      <c r="I127" s="25">
-        <v>0.6771</v>
-      </c>
-      <c r="J127" s="26" t="s">
+      <c r="K127" s="24">
+        <v>8133.0</v>
+      </c>
+      <c r="L127" s="25">
+        <v>0.5174</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="G128" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="K127" s="26">
-        <v>8133.0</v>
-      </c>
-      <c r="L127" s="27">
-        <v>0.5174</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="G128" s="28" t="s">
+      <c r="H128" s="26">
+        <v>63.0</v>
+      </c>
+      <c r="I128" s="27">
+        <v>0.004</v>
+      </c>
+      <c r="J128" s="8"/>
+    </row>
+    <row r="129">
+      <c r="G129" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="H128" s="28">
-        <v>63.0</v>
-      </c>
-      <c r="I128" s="29">
-        <v>0.004</v>
-      </c>
-      <c r="J128" s="8"/>
-    </row>
-    <row r="129">
-      <c r="G129" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="H129" s="28">
+      <c r="H129" s="26">
         <v>493.0</v>
       </c>
-      <c r="I129" s="29">
+      <c r="I129" s="27">
         <v>0.0314</v>
       </c>
     </row>
     <row r="130">
       <c r="F130" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G130" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="H130" s="28">
+        <v>82</v>
+      </c>
+      <c r="G130" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H130" s="26">
         <v>5733.0</v>
       </c>
-      <c r="I130" s="29">
+      <c r="I130" s="27">
         <v>0.3619</v>
       </c>
     </row>
     <row r="131">
       <c r="F131" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G131" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="G131" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="H131" s="28">
+      <c r="H131" s="26">
         <v>7779.0</v>
       </c>
-      <c r="I131" s="29">
+      <c r="I131" s="27">
         <v>0.4786</v>
       </c>
     </row>
     <row r="132">
       <c r="F132" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G132" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="G132" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="H132" s="28">
+      <c r="H132" s="26">
         <v>1652.0</v>
       </c>
-      <c r="I132" s="29">
+      <c r="I132" s="27">
         <v>0.1003</v>
       </c>
     </row>
     <row r="136">
       <c r="F136" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G136" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="G136" s="8" t="s">
+      <c r="H136" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="H136" s="8" t="s">
+      <c r="I136" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="I136" s="8" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="137">
       <c r="F137" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G137" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G137" s="8" t="s">
-        <v>93</v>
-      </c>
       <c r="H137" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="138">
       <c r="F138" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G138" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G138" s="8" t="s">
-        <v>95</v>
-      </c>
       <c r="H138" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I138" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="139">
       <c r="F139" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G139" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G139" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="H139" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I139" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="I139" s="8" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>